<commit_message>
Add disturbance reductions for dead pools. Compile v3.0 rc2.
</commit_message>
<xml_diff>
--- a/deploy/docs/PnET-Succession function worksheet.xlsx
+++ b/deploy/docs/PnET-Succession function worksheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="30" windowWidth="27675" windowHeight="12300" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-12" yWindow="36" windowWidth="27672" windowHeight="12300" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PnET-Succ v. PnET-II" sheetId="9" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <sheet name="Wythers" sheetId="11" r:id="rId9"/>
     <sheet name="fAge" sheetId="13" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Amax" localSheetId="9">#REF!</definedName>
     <definedName name="Amax" localSheetId="0">'PnET-Succ v. PnET-II'!$AD$11</definedName>
@@ -398,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="213">
   <si>
     <t>Shape parameter</t>
   </si>
@@ -1010,9 +1007,6 @@
     <t>350 is the nominal reference concentration</t>
   </si>
   <si>
-    <t>Nominal for ambient CO2</t>
-  </si>
-  <si>
     <t>frad</t>
   </si>
   <si>
@@ -1679,11 +1673,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="240205000"/>
-        <c:axId val="240205784"/>
+        <c:axId val="533647128"/>
+        <c:axId val="533648304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="240205000"/>
+        <c:axId val="533647128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1687,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="240205784"/>
+        <c:crossAx val="533648304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1701,7 +1695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240205784"/>
+        <c:axId val="533648304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1731,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="240205000"/>
+        <c:crossAx val="533647128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1935,11 +1929,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241285600"/>
-        <c:axId val="241277368"/>
+        <c:axId val="533190232"/>
+        <c:axId val="533194936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241285600"/>
+        <c:axId val="533190232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1982,7 +1976,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241277368"/>
+        <c:crossAx val="533194936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1990,7 +1984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241277368"/>
+        <c:axId val="533194936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2041,7 +2035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241285600"/>
+        <c:crossAx val="533190232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2410,11 +2404,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241278936"/>
-        <c:axId val="241283248"/>
+        <c:axId val="533191016"/>
+        <c:axId val="533192976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241278936"/>
+        <c:axId val="533191016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2457,7 +2451,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241283248"/>
+        <c:crossAx val="533192976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2465,7 +2459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241283248"/>
+        <c:axId val="533192976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2516,7 +2510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241278936"/>
+        <c:crossAx val="533191016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2798,11 +2792,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241282072"/>
-        <c:axId val="241279328"/>
+        <c:axId val="533195328"/>
+        <c:axId val="533195720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241282072"/>
+        <c:axId val="533195328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,7 +2839,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241279328"/>
+        <c:crossAx val="533195720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2853,7 +2847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241279328"/>
+        <c:axId val="533195720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2904,7 +2898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241282072"/>
+        <c:crossAx val="533195328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3273,11 +3267,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241283640"/>
-        <c:axId val="241276192"/>
+        <c:axId val="533201992"/>
+        <c:axId val="533200424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241283640"/>
+        <c:axId val="533201992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3375,12 +3369,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241276192"/>
+        <c:crossAx val="533200424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241276192"/>
+        <c:axId val="533200424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -3468,7 +3462,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241283640"/>
+        <c:crossAx val="533201992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3787,11 +3781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241279720"/>
-        <c:axId val="241280112"/>
+        <c:axId val="533201208"/>
+        <c:axId val="533201600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241279720"/>
+        <c:axId val="533201208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3889,12 +3883,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241280112"/>
+        <c:crossAx val="533201600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241280112"/>
+        <c:axId val="533201600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3981,7 +3975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241279720"/>
+        <c:crossAx val="533201208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4290,11 +4284,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241280504"/>
-        <c:axId val="241284816"/>
+        <c:axId val="533199248"/>
+        <c:axId val="533200032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241280504"/>
+        <c:axId val="533199248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4392,12 +4386,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241284816"/>
+        <c:crossAx val="533200032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241284816"/>
+        <c:axId val="533200032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4484,7 +4478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241280504"/>
+        <c:crossAx val="533199248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4939,11 +4933,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241281288"/>
-        <c:axId val="241284424"/>
+        <c:axId val="536484040"/>
+        <c:axId val="536482080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241281288"/>
+        <c:axId val="536484040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5041,12 +5035,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241284424"/>
+        <c:crossAx val="536482080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241284424"/>
+        <c:axId val="536482080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5133,7 +5127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241281288"/>
+        <c:crossAx val="536484040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5417,11 +5411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241286776"/>
-        <c:axId val="241287168"/>
+        <c:axId val="536478552"/>
+        <c:axId val="536485216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241286776"/>
+        <c:axId val="536478552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5519,12 +5513,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241287168"/>
+        <c:crossAx val="536485216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241287168"/>
+        <c:axId val="536485216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5611,7 +5605,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241286776"/>
+        <c:crossAx val="536478552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5920,11 +5914,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="241287560"/>
-        <c:axId val="241289912"/>
+        <c:axId val="536488744"/>
+        <c:axId val="536485608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="241287560"/>
+        <c:axId val="536488744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6022,12 +6016,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241289912"/>
+        <c:crossAx val="536485608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241289912"/>
+        <c:axId val="536485608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6114,7 +6108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241287560"/>
+        <c:crossAx val="536488744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6314,31 +6308,31 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>365</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>450</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>600</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>650</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>700</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>750</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6356,31 +6350,31 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>197</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>190</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>170</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>150</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>130</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6426,31 +6420,31 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>365</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>450</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>550</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>600</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>650</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>700</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>750</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6462,37 +6456,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>301.5</c:v>
+                  <c:v>297.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>299.55</c:v>
+                  <c:v>302.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>298.5</c:v>
+                  <c:v>305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>297</c:v>
+                  <c:v>307.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>295.5</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>294</c:v>
+                  <c:v>312.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>292.5</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>291</c:v>
+                  <c:v>317.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>289.5</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>288</c:v>
+                  <c:v>322.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6508,11 +6502,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241289520"/>
-        <c:axId val="241288344"/>
+        <c:axId val="536480512"/>
+        <c:axId val="536486000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241289520"/>
+        <c:axId val="536480512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6611,7 +6605,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241288344"/>
+        <c:crossAx val="536486000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6619,7 +6613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241288344"/>
+        <c:axId val="536486000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6731,7 +6725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241289520"/>
+        <c:crossAx val="536480512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7078,11 +7072,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="240206568"/>
-        <c:axId val="240206960"/>
+        <c:axId val="533647912"/>
+        <c:axId val="533193760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="240206568"/>
+        <c:axId val="533647912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7092,7 +7086,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="240206960"/>
+        <c:crossAx val="533193760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7100,7 +7094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240206960"/>
+        <c:axId val="533193760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7136,7 +7130,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="240206568"/>
+        <c:crossAx val="533647912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7172,7 +7166,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7343,11 +7336,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="241289128"/>
-        <c:axId val="241290304"/>
+        <c:axId val="536486392"/>
+        <c:axId val="536488352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241289128"/>
+        <c:axId val="536486392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7379,7 +7372,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7446,7 +7438,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241290304"/>
+        <c:crossAx val="536488352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7454,7 +7446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241290304"/>
+        <c:axId val="536488352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7501,7 +7493,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7562,7 +7553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241289128"/>
+        <c:crossAx val="536486392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7576,7 +7567,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7683,7 +7673,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7952,11 +7941,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239043736"/>
-        <c:axId val="545604336"/>
+        <c:axId val="536477376"/>
+        <c:axId val="536486784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239043736"/>
+        <c:axId val="536477376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7993,7 +7982,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8060,7 +8048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545604336"/>
+        <c:crossAx val="536486784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8068,7 +8056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545604336"/>
+        <c:axId val="536486784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8115,7 +8103,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8176,7 +8163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239043736"/>
+        <c:crossAx val="536477376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8190,7 +8177,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8541,11 +8527,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="547308152"/>
-        <c:axId val="706180560"/>
+        <c:axId val="536489136"/>
+        <c:axId val="536481688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="547308152"/>
+        <c:axId val="536489136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8588,7 +8574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="706180560"/>
+        <c:crossAx val="536481688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8596,7 +8582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="706180560"/>
+        <c:axId val="536481688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8647,7 +8633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="547308152"/>
+        <c:crossAx val="536489136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8775,7 +8761,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9034,11 +9019,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="545596888"/>
-        <c:axId val="545600808"/>
+        <c:axId val="536487960"/>
+        <c:axId val="536476984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="545596888"/>
+        <c:axId val="536487960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9081,7 +9066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545600808"/>
+        <c:crossAx val="536476984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9089,7 +9074,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545600808"/>
+        <c:axId val="536476984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9140,7 +9125,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545596888"/>
+        <c:crossAx val="536487960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9229,7 +9214,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9486,11 +9470,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="545600416"/>
-        <c:axId val="545605120"/>
+        <c:axId val="536481296"/>
+        <c:axId val="536482472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="545600416"/>
+        <c:axId val="536481296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9533,7 +9517,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545605120"/>
+        <c:crossAx val="536482472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9541,7 +9525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545605120"/>
+        <c:axId val="536482472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9592,7 +9576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545600416"/>
+        <c:crossAx val="536481296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9606,7 +9590,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9713,7 +9696,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9970,11 +9952,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="545603552"/>
-        <c:axId val="545599632"/>
+        <c:axId val="536479336"/>
+        <c:axId val="536479728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="545603552"/>
+        <c:axId val="536479336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10017,7 +9999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545599632"/>
+        <c:crossAx val="536479728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10025,7 +10007,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545599632"/>
+        <c:axId val="536479728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10076,7 +10058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545603552"/>
+        <c:crossAx val="536479336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10090,7 +10072,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10197,7 +10178,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10376,11 +10356,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="545601200"/>
-        <c:axId val="545598848"/>
+        <c:axId val="536483256"/>
+        <c:axId val="536483648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="545601200"/>
+        <c:axId val="536483256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10422,7 +10402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545598848"/>
+        <c:crossAx val="536483648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10430,7 +10410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545598848"/>
+        <c:axId val="536483648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10481,7 +10461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545601200"/>
+        <c:crossAx val="536483256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10495,7 +10475,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10602,7 +10581,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10893,11 +10871,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="545601984"/>
-        <c:axId val="545601592"/>
+        <c:axId val="536495800"/>
+        <c:axId val="536490312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="545601984"/>
+        <c:axId val="536495800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10934,7 +10912,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11001,7 +10978,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545601592"/>
+        <c:crossAx val="536490312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11009,7 +10986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545601592"/>
+        <c:axId val="536490312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11055,7 +11032,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11116,7 +11092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545601984"/>
+        <c:crossAx val="536495800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11130,7 +11106,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11462,11 +11437,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239050792"/>
-        <c:axId val="239051184"/>
+        <c:axId val="533197680"/>
+        <c:axId val="533196896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239050792"/>
+        <c:axId val="533197680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11476,7 +11451,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239051184"/>
+        <c:crossAx val="533196896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11484,7 +11459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239051184"/>
+        <c:axId val="533196896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11520,7 +11495,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239050792"/>
+        <c:crossAx val="533197680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11806,11 +11781,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239051576"/>
-        <c:axId val="239052752"/>
+        <c:axId val="533189448"/>
+        <c:axId val="533194152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239051576"/>
+        <c:axId val="533189448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11820,7 +11795,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239052752"/>
+        <c:crossAx val="533194152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11828,7 +11803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239052752"/>
+        <c:axId val="533194152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11860,7 +11835,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239051576"/>
+        <c:crossAx val="533189448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12146,11 +12121,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239042952"/>
-        <c:axId val="239049224"/>
+        <c:axId val="533188272"/>
+        <c:axId val="533188664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239042952"/>
+        <c:axId val="533188272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12160,7 +12135,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239049224"/>
+        <c:crossAx val="533188664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12168,7 +12143,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239049224"/>
+        <c:axId val="533188664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12197,7 +12172,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="239042952"/>
+        <c:crossAx val="533188272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12538,11 +12513,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239041776"/>
-        <c:axId val="239044912"/>
+        <c:axId val="533194544"/>
+        <c:axId val="533191800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239041776"/>
+        <c:axId val="533194544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12585,7 +12560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239044912"/>
+        <c:crossAx val="533191800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12593,7 +12568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="239044912"/>
+        <c:axId val="533191800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12644,7 +12619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239041776"/>
+        <c:crossAx val="533194544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12827,11 +12802,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="239046872"/>
-        <c:axId val="241278544"/>
+        <c:axId val="533187488"/>
+        <c:axId val="533187880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="239046872"/>
+        <c:axId val="533187488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12873,7 +12848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241278544"/>
+        <c:crossAx val="533187880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12881,7 +12856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241278544"/>
+        <c:axId val="533187880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12932,7 +12907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239046872"/>
+        <c:crossAx val="533187488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13301,11 +13276,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241285208"/>
-        <c:axId val="241275800"/>
+        <c:axId val="533190624"/>
+        <c:axId val="533189056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241285208"/>
+        <c:axId val="533190624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13348,7 +13323,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241275800"/>
+        <c:crossAx val="533189056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13356,7 +13331,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241275800"/>
+        <c:axId val="533189056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13407,7 +13382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241285208"/>
+        <c:crossAx val="533190624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13807,11 +13782,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241282464"/>
-        <c:axId val="241276584"/>
+        <c:axId val="533192584"/>
+        <c:axId val="533189840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241282464"/>
+        <c:axId val="533192584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13854,7 +13829,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241276584"/>
+        <c:crossAx val="533189840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13862,7 +13837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241276584"/>
+        <c:axId val="533189840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13913,7 +13888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241282464"/>
+        <c:crossAx val="533192584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26949,13 +26924,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -27157,221 +27132,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>exp multiplier</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>lin multiplier</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>expFolN</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>linFolN</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>0</v>
-          </cell>
-          <cell r="B2">
-            <v>0.30000000000000004</v>
-          </cell>
-          <cell r="C2">
-            <v>0.30000000000000004</v>
-          </cell>
-          <cell r="D2">
-            <v>0.58200000000000007</v>
-          </cell>
-          <cell r="E2">
-            <v>0.58200000000000007</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>0.1</v>
-          </cell>
-          <cell r="B3">
-            <v>0.31000000000000005</v>
-          </cell>
-          <cell r="C3">
-            <v>0.44000000000000006</v>
-          </cell>
-          <cell r="D3">
-            <v>0.60140000000000005</v>
-          </cell>
-          <cell r="E3">
-            <v>0.85360000000000014</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>0.2</v>
-          </cell>
-          <cell r="B4">
-            <v>0.34000000000000008</v>
-          </cell>
-          <cell r="C4">
-            <v>0.58000000000000007</v>
-          </cell>
-          <cell r="D4">
-            <v>0.65960000000000019</v>
-          </cell>
-          <cell r="E4">
-            <v>1.1252000000000002</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>0.3</v>
-          </cell>
-          <cell r="B5">
-            <v>0.39</v>
-          </cell>
-          <cell r="C5">
-            <v>0.72</v>
-          </cell>
-          <cell r="D5">
-            <v>0.75660000000000005</v>
-          </cell>
-          <cell r="E5">
-            <v>1.3967999999999998</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>0.4</v>
-          </cell>
-          <cell r="B6">
-            <v>0.46000000000000008</v>
-          </cell>
-          <cell r="C6">
-            <v>0.86</v>
-          </cell>
-          <cell r="D6">
-            <v>0.89240000000000008</v>
-          </cell>
-          <cell r="E6">
-            <v>1.6683999999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>0.5</v>
-          </cell>
-          <cell r="B7">
-            <v>0.55000000000000004</v>
-          </cell>
-          <cell r="C7">
-            <v>1</v>
-          </cell>
-          <cell r="D7">
-            <v>1.0669999999999999</v>
-          </cell>
-          <cell r="E7">
-            <v>1.94</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>0.6</v>
-          </cell>
-          <cell r="B8">
-            <v>0.66</v>
-          </cell>
-          <cell r="C8">
-            <v>1.1400000000000001</v>
-          </cell>
-          <cell r="D8">
-            <v>1.2804</v>
-          </cell>
-          <cell r="E8">
-            <v>2.2116000000000002</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>0.7</v>
-          </cell>
-          <cell r="B9">
-            <v>0.79</v>
-          </cell>
-          <cell r="C9">
-            <v>1.2799999999999998</v>
-          </cell>
-          <cell r="D9">
-            <v>1.5326</v>
-          </cell>
-          <cell r="E9">
-            <v>2.4831999999999996</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>0.8</v>
-          </cell>
-          <cell r="B10">
-            <v>0.94000000000000017</v>
-          </cell>
-          <cell r="C10">
-            <v>1.42</v>
-          </cell>
-          <cell r="D10">
-            <v>1.8236000000000003</v>
-          </cell>
-          <cell r="E10">
-            <v>2.7547999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>0.9</v>
-          </cell>
-          <cell r="B11">
-            <v>1.1100000000000001</v>
-          </cell>
-          <cell r="C11">
-            <v>1.56</v>
-          </cell>
-          <cell r="D11">
-            <v>2.1534</v>
-          </cell>
-          <cell r="E11">
-            <v>3.0264000000000002</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>1</v>
-          </cell>
-          <cell r="B12">
-            <v>1.3</v>
-          </cell>
-          <cell r="C12">
-            <v>1.7</v>
-          </cell>
-          <cell r="D12">
-            <v>2.5219999999999998</v>
-          </cell>
-          <cell r="E12">
-            <v>3.298</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -27665,43 +27425,43 @@
       <selection activeCell="AI33" sqref="AI33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="6" width="9.140625" style="27"/>
+    <col min="1" max="6" width="9.109375" style="27"/>
     <col min="7" max="8" width="0" style="27" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="27"/>
-    <col min="10" max="10" width="14.42578125" style="27" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="27"/>
+    <col min="10" max="10" width="14.44140625" style="27" customWidth="1"/>
     <col min="11" max="11" width="15" style="27" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="27" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="27" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="27" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" style="27" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="27" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="27" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="27" customWidth="1"/>
-    <col min="19" max="20" width="13.7109375" style="27" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="27" customWidth="1"/>
-    <col min="22" max="22" width="15.28515625" style="27" customWidth="1"/>
-    <col min="23" max="23" width="19.42578125" style="27" customWidth="1"/>
-    <col min="24" max="24" width="21.42578125" style="27" customWidth="1"/>
-    <col min="25" max="25" width="23.28515625" style="27" customWidth="1"/>
-    <col min="26" max="26" width="20.5703125" style="27" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="27" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" style="27" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="27" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" style="27" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="13.44140625" style="27" customWidth="1"/>
+    <col min="18" max="18" width="19.109375" style="27" customWidth="1"/>
+    <col min="19" max="20" width="13.6640625" style="27" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="27" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" style="27" customWidth="1"/>
+    <col min="23" max="23" width="19.44140625" style="27" customWidth="1"/>
+    <col min="24" max="24" width="21.44140625" style="27" customWidth="1"/>
+    <col min="25" max="25" width="23.33203125" style="27" customWidth="1"/>
+    <col min="26" max="26" width="20.5546875" style="27" customWidth="1"/>
     <col min="27" max="27" width="7" style="27" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" style="27" customWidth="1"/>
-    <col min="29" max="30" width="9.140625" style="27"/>
-    <col min="31" max="31" width="13.7109375" style="27" customWidth="1"/>
-    <col min="32" max="32" width="9.140625" style="27"/>
-    <col min="33" max="33" width="14.140625" style="27" customWidth="1"/>
-    <col min="34" max="34" width="10.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.140625" style="27"/>
-    <col min="36" max="36" width="16.28515625" style="27" customWidth="1"/>
-    <col min="37" max="37" width="16.85546875" style="27" customWidth="1"/>
-    <col min="38" max="43" width="9.140625" style="27"/>
-    <col min="44" max="44" width="11.7109375" style="27" customWidth="1"/>
-    <col min="45" max="16384" width="9.140625" style="27"/>
+    <col min="28" max="28" width="14.88671875" style="27" customWidth="1"/>
+    <col min="29" max="30" width="9.109375" style="27"/>
+    <col min="31" max="31" width="13.6640625" style="27" customWidth="1"/>
+    <col min="32" max="32" width="9.109375" style="27"/>
+    <col min="33" max="33" width="14.109375" style="27" customWidth="1"/>
+    <col min="34" max="34" width="10.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.109375" style="27"/>
+    <col min="36" max="36" width="16.33203125" style="27" customWidth="1"/>
+    <col min="37" max="37" width="16.88671875" style="27" customWidth="1"/>
+    <col min="38" max="43" width="9.109375" style="27"/>
+    <col min="44" max="44" width="11.6640625" style="27" customWidth="1"/>
+    <col min="45" max="16384" width="9.109375" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="15.75" thickBot="1">
+    <row r="1" spans="1:57" ht="15" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>58</v>
       </c>
@@ -28944,7 +28704,7 @@
       <c r="AH12" s="50"/>
       <c r="AI12" s="50"/>
     </row>
-    <row r="13" spans="1:57" ht="15.75" thickBot="1">
+    <row r="13" spans="1:57" ht="15" thickBot="1">
       <c r="B13" s="27">
         <v>40</v>
       </c>
@@ -29166,7 +28926,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:49" ht="15.75" thickBot="1">
+    <row r="19" spans="1:49" ht="15" thickBot="1">
       <c r="G19" s="27" t="s">
         <v>106</v>
       </c>
@@ -29202,7 +28962,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:49" ht="15.75" thickBot="1">
+    <row r="20" spans="1:49" ht="15" thickBot="1">
       <c r="A20" s="27" t="s">
         <v>55</v>
       </c>
@@ -29280,7 +29040,7 @@
       <c r="AV20" s="8"/>
       <c r="AW20" s="8"/>
     </row>
-    <row r="21" spans="1:49" ht="15.75" thickBot="1">
+    <row r="21" spans="1:49" ht="15" thickBot="1">
       <c r="G21" s="11">
         <f>IF(Tday &lt;0,0.61078 * EXP(21.87456 * Tday / (Tday + 265.5)),0.61078 * EXP(17.26939 * Tday / (Tday + 237.3)))</f>
         <v>0.61077999999999999</v>
@@ -29374,7 +29134,7 @@
       <c r="AV21" s="8"/>
       <c r="AW21" s="8"/>
     </row>
-    <row r="22" spans="1:49" ht="15.75" thickBot="1">
+    <row r="22" spans="1:49" ht="15" thickBot="1">
       <c r="G22" s="11">
         <f>IF(E3 &lt;0,0.61078 * EXP(21.87456 * E3 / (E3 + 265.5)),0.61078 * EXP(17.26939 * E3 / (E3 + 237.3)))</f>
         <v>0.87227141748882542</v>
@@ -29459,7 +29219,7 @@
       <c r="AV22" s="8"/>
       <c r="AW22" s="8"/>
     </row>
-    <row r="23" spans="1:49" ht="15.75" thickBot="1">
+    <row r="23" spans="1:49" ht="15" thickBot="1">
       <c r="G23" s="11">
         <f t="shared" ref="G23:G32" si="31">IF(E4 &lt;0,0.61078 * EXP(21.87456 * E4 / (E4 + 265.5)),0.61078 * EXP(17.26939 * E4 / (E4 + 237.3)))</f>
         <v>1.2278921229539039</v>
@@ -29545,7 +29305,7 @@
       <c r="AV23" s="8"/>
       <c r="AW23" s="8"/>
     </row>
-    <row r="24" spans="1:49" ht="15.75" thickBot="1">
+    <row r="24" spans="1:49" ht="15" thickBot="1">
       <c r="G24" s="11">
         <f t="shared" si="31"/>
         <v>1.7052285488209411</v>
@@ -29634,7 +29394,7 @@
       <c r="AV24" s="8"/>
       <c r="AW24" s="8"/>
     </row>
-    <row r="25" spans="1:49" ht="15.75" thickBot="1">
+    <row r="25" spans="1:49" ht="15" thickBot="1">
       <c r="G25" s="11">
         <f t="shared" si="31"/>
         <v>2.3380938419374377</v>
@@ -29727,7 +29487,7 @@
       <c r="AV25" s="8"/>
       <c r="AW25" s="8"/>
     </row>
-    <row r="26" spans="1:49" ht="15.75" thickBot="1">
+    <row r="26" spans="1:49" ht="15" thickBot="1">
       <c r="G26" s="11">
         <f t="shared" si="31"/>
         <v>3.1674898302368564</v>
@@ -29819,7 +29579,7 @@
       <c r="AV26" s="8"/>
       <c r="AW26" s="8"/>
     </row>
-    <row r="27" spans="1:49" ht="15.75" thickBot="1">
+    <row r="27" spans="1:49" ht="15" thickBot="1">
       <c r="G27" s="11">
         <f t="shared" si="31"/>
         <v>4.2426356531114431</v>
@@ -29903,7 +29663,7 @@
       <c r="AV27" s="8"/>
       <c r="AW27" s="8"/>
     </row>
-    <row r="28" spans="1:49" ht="15.75" thickBot="1">
+    <row r="28" spans="1:49" ht="15" thickBot="1">
       <c r="G28" s="11">
         <f t="shared" si="31"/>
         <v>5.6220563085635584</v>
@@ -29987,7 +29747,7 @@
       <c r="AV28" s="8"/>
       <c r="AW28" s="8"/>
     </row>
-    <row r="29" spans="1:49" ht="15.75" thickBot="1">
+    <row r="29" spans="1:49" ht="15" thickBot="1">
       <c r="G29" s="11">
         <f t="shared" si="31"/>
         <v>7.3747231460360023</v>
@@ -30073,7 +29833,7 @@
       <c r="AV29" s="8"/>
       <c r="AW29" s="8"/>
     </row>
-    <row r="30" spans="1:49" ht="15.75" thickBot="1">
+    <row r="30" spans="1:49" ht="15" thickBot="1">
       <c r="G30" s="11">
         <f t="shared" si="31"/>
         <v>9.5812372781996284</v>
@@ -30169,7 +29929,7 @@
       <c r="AV30" s="8"/>
       <c r="AW30" s="8"/>
     </row>
-    <row r="31" spans="1:49" ht="15.75" thickBot="1">
+    <row r="31" spans="1:49" ht="15" thickBot="1">
       <c r="G31" s="11">
         <f t="shared" si="31"/>
         <v>12.335046017492973</v>
@@ -30258,7 +30018,7 @@
       <c r="AV31" s="8"/>
       <c r="AW31" s="8"/>
     </row>
-    <row r="32" spans="1:49" ht="15.75" thickBot="1">
+    <row r="32" spans="1:49" ht="15" thickBot="1">
       <c r="G32" s="12">
         <f t="shared" si="31"/>
         <v>15.743681776119971</v>
@@ -30944,14 +30704,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="27"/>
-    <col min="2" max="2" width="12.42578125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="27"/>
-    <col min="5" max="5" width="12.28515625" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="9.109375" style="27"/>
+    <col min="2" max="2" width="12.44140625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="27"/>
+    <col min="5" max="5" width="12.33203125" style="27" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -30992,7 +30752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75">
+    <row r="4" spans="1:6" ht="15.6">
       <c r="A4" s="27">
         <v>20</v>
       </c>
@@ -31289,7 +31049,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -31380,13 +31140,13 @@
       <selection activeCell="P2" sqref="P2:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="27"/>
-    <col min="14" max="14" width="9.140625" style="27"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="27"/>
+    <col min="14" max="14" width="9.109375" style="27"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -32765,14 +32525,14 @@
       <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="8" max="8" width="9.140625" style="27"/>
-    <col min="9" max="17" width="9.140625" style="4"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="4"/>
-    <col min="25" max="25" width="10.42578125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="27"/>
+    <col min="9" max="17" width="9.109375" style="4"/>
+    <col min="18" max="18" width="12.5546875" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" style="4"/>
+    <col min="25" max="25" width="10.44140625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -32828,7 +32588,7 @@
       <c r="T1" s="31"/>
       <c r="U1" s="31"/>
       <c r="V1" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
@@ -32899,7 +32659,7 @@
       <c r="T2" s="31"/>
       <c r="U2" s="31"/>
       <c r="V2" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
@@ -32976,7 +32736,7 @@
       </c>
       <c r="U3" s="31"/>
       <c r="V3" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -34040,14 +33800,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" style="27" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="27"/>
+    <col min="2" max="16384" width="9.109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -34087,12 +33847,12 @@
         <v>-0.2</v>
       </c>
       <c r="C3" s="27">
-        <v>-0.03</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>198</v>
@@ -34111,7 +33871,7 @@
       </c>
       <c r="C7" s="27">
         <f>C$3*A7 + (C$2 - (350*C$3))</f>
-        <v>301.5</v>
+        <v>297.5</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -34135,127 +33895,125 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="27">
-        <v>365</v>
-      </c>
-      <c r="B9" s="31">
+        <v>400</v>
+      </c>
+      <c r="B9" s="27">
         <f t="shared" si="0"/>
-        <v>197</v>
-      </c>
-      <c r="C9" s="31">
+        <v>190</v>
+      </c>
+      <c r="C9" s="27">
         <f t="shared" si="1"/>
-        <v>299.55</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>200</v>
+        <v>302.5</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="27">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="B10" s="27">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C10" s="27">
         <f t="shared" si="1"/>
-        <v>298.5</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="27">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="B11" s="27">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C11" s="27">
         <f t="shared" si="1"/>
-        <v>297</v>
+        <v>307.5</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="27">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="B12" s="27">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C12" s="27">
         <f t="shared" si="1"/>
-        <v>295.5</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="27">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="B13" s="27">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C13" s="27">
         <f t="shared" si="1"/>
-        <v>294</v>
+        <v>312.5</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="27">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="B14" s="27">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C14" s="27">
         <f t="shared" si="1"/>
-        <v>292.5</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="27">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="B15" s="27">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C15" s="27">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>317.5</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="27">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="B16" s="27">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C16" s="27">
         <f t="shared" si="1"/>
-        <v>289.5</v>
+        <v>320</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="27">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="B17" s="27">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C17" s="27">
         <f t="shared" si="1"/>
-        <v>288</v>
+        <v>322.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -34267,9 +34025,9 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="27"/>
+    <col min="2" max="2" width="9.109375" style="27"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -34599,30 +34357,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="59" t="s">
         <v>203</v>
-      </c>
-      <c r="F1" s="59" t="s">
-        <v>204</v>
       </c>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
@@ -34640,11 +34398,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="27">
-        <f>A2*$E$2+$D$2</f>
+        <f t="shared" ref="B2:B12" si="0">A2*$E$2+$D$2</f>
         <v>0.8</v>
       </c>
       <c r="C2" s="27">
-        <f>$F$2*B2</f>
+        <f t="shared" ref="C2:C12" si="1">$F$2*B2</f>
         <v>1.6</v>
       </c>
       <c r="D2" s="27">
@@ -34672,11 +34430,11 @@
         <v>0.1</v>
       </c>
       <c r="B3" s="27">
-        <f>A3*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>0.84000000000000008</v>
       </c>
       <c r="C3" s="27">
-        <f>$F$2*B3</f>
+        <f t="shared" si="1"/>
         <v>1.6800000000000002</v>
       </c>
       <c r="D3" s="27"/>
@@ -34698,11 +34456,11 @@
         <v>0.2</v>
       </c>
       <c r="B4" s="27">
-        <f>A4*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>0.88000000000000012</v>
       </c>
       <c r="C4" s="27">
-        <f>$F$2*B4</f>
+        <f t="shared" si="1"/>
         <v>1.7600000000000002</v>
       </c>
       <c r="D4" s="27"/>
@@ -34724,11 +34482,11 @@
         <v>0.3</v>
       </c>
       <c r="B5" s="27">
-        <f>A5*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
       <c r="C5" s="27">
-        <f>$F$2*B5</f>
+        <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
       <c r="D5" s="27"/>
@@ -34750,11 +34508,11 @@
         <v>0.4</v>
       </c>
       <c r="B6" s="27">
-        <f>A6*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>0.96000000000000008</v>
       </c>
       <c r="C6" s="27">
-        <f>$F$2*B6</f>
+        <f t="shared" si="1"/>
         <v>1.9200000000000002</v>
       </c>
       <c r="D6" s="27"/>
@@ -34776,11 +34534,11 @@
         <v>0.5</v>
       </c>
       <c r="B7" s="27">
-        <f>A7*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C7" s="27">
-        <f>$F$2*B7</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D7" s="27"/>
@@ -34802,11 +34560,11 @@
         <v>0.6</v>
       </c>
       <c r="B8" s="27">
-        <f>A8*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>1.04</v>
       </c>
       <c r="C8" s="27">
-        <f>$F$2*B8</f>
+        <f t="shared" si="1"/>
         <v>2.08</v>
       </c>
       <c r="D8" s="27"/>
@@ -34828,11 +34586,11 @@
         <v>0.7</v>
       </c>
       <c r="B9" s="27">
-        <f>A9*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
       <c r="C9" s="27">
-        <f>$F$2*B9</f>
+        <f t="shared" si="1"/>
         <v>2.16</v>
       </c>
       <c r="D9" s="27"/>
@@ -34854,11 +34612,11 @@
         <v>0.8</v>
       </c>
       <c r="B10" s="27">
-        <f>A10*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="C10" s="27">
-        <f>$F$2*B10</f>
+        <f t="shared" si="1"/>
         <v>2.2400000000000002</v>
       </c>
       <c r="D10" s="27"/>
@@ -34880,11 +34638,11 @@
         <v>0.9</v>
       </c>
       <c r="B11" s="27">
-        <f>A11*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>1.1600000000000001</v>
       </c>
       <c r="C11" s="27">
-        <f>$F$2*B11</f>
+        <f t="shared" si="1"/>
         <v>2.3200000000000003</v>
       </c>
       <c r="D11" s="27"/>
@@ -34906,11 +34664,11 @@
         <v>1</v>
       </c>
       <c r="B12" s="27">
-        <f>A12*$E$2+$D$2</f>
+        <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="C12" s="27">
-        <f>$F$2*B12</f>
+        <f t="shared" si="1"/>
         <v>2.4000000000000004</v>
       </c>
       <c r="D12" s="27"/>
@@ -35301,20 +35059,20 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -35349,7 +35107,7 @@
         <v>0.84029689765843141</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.6">
       <c r="A5" s="27">
         <f t="shared" si="1"/>
         <v>4300</v>
@@ -35615,18 +35373,18 @@
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="27"/>
-    <col min="3" max="3" width="10.28515625" style="27" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="27"/>
+    <col min="3" max="3" width="10.33203125" style="27" customWidth="1"/>
     <col min="4" max="4" width="11" style="27" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="27" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="27"/>
-    <col min="9" max="9" width="10.140625" style="27" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="27"/>
+    <col min="5" max="5" width="11.5546875" style="27" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="27" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="27"/>
+    <col min="9" max="9" width="10.109375" style="27" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">

</xml_diff>

<commit_message>
Add PsnTMax species parameter. Modify DTempResponse function to use PsnTMax.
</commit_message>
<xml_diff>
--- a/deploy/docs/PnET-Succession function worksheet.xlsx
+++ b/deploy/docs/PnET-Succession function worksheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egustafson\Documents\USERDOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BRM\LANDIS_II\GitCode\Extension-PnET-Succession\deploy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="36" windowWidth="27672" windowHeight="12300" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="30" windowWidth="27675" windowHeight="12300" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PnET-Succ v. PnET-II" sheetId="9" r:id="rId1"/>
@@ -395,7 +395,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="214">
   <si>
     <t>Shape parameter</t>
   </si>
@@ -1045,6 +1045,9 @@
   <si>
     <t>AdjFolN</t>
   </si>
+  <si>
+    <t>used for dTemp calc</t>
+  </si>
 </sst>
 </file>
 
@@ -1673,11 +1676,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533647128"/>
-        <c:axId val="533648304"/>
+        <c:axId val="395138416"/>
+        <c:axId val="395136064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533647128"/>
+        <c:axId val="395138416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1687,7 +1690,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533648304"/>
+        <c:crossAx val="395136064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1695,7 +1698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533648304"/>
+        <c:axId val="395136064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1734,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533647128"/>
+        <c:crossAx val="395138416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1767,6 +1770,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1830,7 +1834,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1875,45 +1879,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$V$2:$V$13</c:f>
+              <c:f>DTemp!$V$3:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>0.67463601518224492</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.95407940233607225</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.3492720303644898</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.9081588046721443</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2.6985440607289797</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>3.8163176093442885</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>5.3970881214579594</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7.6326352186885771</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>10.794176242915919</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>15.265270437377154</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>21.588352485831837</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>30.530540874754308</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43.176704971663675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1929,11 +1933,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533190232"/>
-        <c:axId val="533194936"/>
+        <c:axId val="395672872"/>
+        <c:axId val="395673264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533190232"/>
+        <c:axId val="395672872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +1980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533194936"/>
+        <c:crossAx val="395673264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1984,7 +1988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533194936"/>
+        <c:axId val="395673264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2035,7 +2039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533190232"/>
+        <c:crossAx val="395672872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2124,6 +2128,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2187,7 +2192,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2232,27 +2237,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$O$2:$O$13</c:f>
+              <c:f>DTemp!$O$3:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.109296798542994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6790800556289511</c:v>
+                  <c:v>14.211684507044843</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.896595013127973</c:v>
+                  <c:v>18.223683789037992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.520072192029389</c:v>
+                  <c:v>20.033845653446861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.402505512568759</c:v>
+                  <c:v>19.530227445558033</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.795983973062672</c:v>
+                  <c:v>16.683734974746255</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>14.862789772321459</c:v>
@@ -2305,7 +2310,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2350,36 +2355,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$P$2:$P$13</c:f>
+              <c:f>DTemp!$P$3:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.2587741279452471</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6790800556289511</c:v>
+                  <c:v>11.35999781319703</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.896595013127973</c:v>
+                  <c:v>15.220917710162411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.520072192029389</c:v>
+                  <c:v>17.708488568671783</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.402505512568759</c:v>
+                  <c:v>18.628015851605625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.465066915712335</c:v>
+                  <c:v>17.726468410667898</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.897462199121927</c:v>
+                  <c:v>14.340269819388283</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.573230783432443</c:v>
+                  <c:v>7.5748659504316729</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83298962341503313</c:v>
+                  <c:v>0.85633610993066933</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2404,11 +2409,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533191016"/>
-        <c:axId val="533192976"/>
+        <c:axId val="395668168"/>
+        <c:axId val="395674832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533191016"/>
+        <c:axId val="395668168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2456,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533192976"/>
+        <c:crossAx val="395674832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2459,7 +2464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533192976"/>
+        <c:axId val="395674832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2510,7 +2515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533191016"/>
+        <c:crossAx val="395668168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2524,6 +2529,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2630,6 +2636,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2693,7 +2700,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2738,7 +2745,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$I$2:$I$13</c:f>
+              <c:f>DTemp!$I$3:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -2792,11 +2799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533195328"/>
-        <c:axId val="533195720"/>
+        <c:axId val="395667384"/>
+        <c:axId val="395137240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533195328"/>
+        <c:axId val="395667384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,7 +2846,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533195720"/>
+        <c:crossAx val="395137240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2847,7 +2854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533195720"/>
+        <c:axId val="395137240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2898,7 +2905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533195328"/>
+        <c:crossAx val="395667384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3267,11 +3274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="533201992"/>
-        <c:axId val="533200424"/>
+        <c:axId val="395135280"/>
+        <c:axId val="395139592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="533201992"/>
+        <c:axId val="395135280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3369,12 +3376,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533200424"/>
+        <c:crossAx val="395139592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="533200424"/>
+        <c:axId val="395139592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350"/>
@@ -3462,7 +3469,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533201992"/>
+        <c:crossAx val="395135280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3781,11 +3788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="533201208"/>
-        <c:axId val="533201600"/>
+        <c:axId val="396614104"/>
+        <c:axId val="396615672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="533201208"/>
+        <c:axId val="396614104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3883,12 +3890,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533201600"/>
+        <c:crossAx val="396615672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="533201600"/>
+        <c:axId val="396615672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3975,7 +3982,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533201208"/>
+        <c:crossAx val="396614104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4284,11 +4291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="533199248"/>
-        <c:axId val="533200032"/>
+        <c:axId val="396614888"/>
+        <c:axId val="396619592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="533199248"/>
+        <c:axId val="396614888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4386,12 +4393,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533200032"/>
+        <c:crossAx val="396619592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="533200032"/>
+        <c:axId val="396619592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4478,7 +4485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533199248"/>
+        <c:crossAx val="396614888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4933,11 +4940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="536484040"/>
-        <c:axId val="536482080"/>
+        <c:axId val="396616848"/>
+        <c:axId val="396612928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="536484040"/>
+        <c:axId val="396616848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5035,12 +5042,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536482080"/>
+        <c:crossAx val="396612928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="536482080"/>
+        <c:axId val="396612928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5127,7 +5134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536484040"/>
+        <c:crossAx val="396616848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5411,11 +5418,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="536478552"/>
-        <c:axId val="536485216"/>
+        <c:axId val="396614496"/>
+        <c:axId val="396613712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="536478552"/>
+        <c:axId val="396614496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5513,12 +5520,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536485216"/>
+        <c:crossAx val="396613712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="536485216"/>
+        <c:axId val="396613712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5605,7 +5612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536478552"/>
+        <c:crossAx val="396614496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5914,11 +5921,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="536488744"/>
-        <c:axId val="536485608"/>
+        <c:axId val="396616064"/>
+        <c:axId val="396616456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="536488744"/>
+        <c:axId val="396616064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6016,12 +6023,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536485608"/>
+        <c:crossAx val="396616456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="536485608"/>
+        <c:axId val="396616456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6108,7 +6115,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536488744"/>
+        <c:crossAx val="396616064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6502,11 +6509,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536480512"/>
-        <c:axId val="536486000"/>
+        <c:axId val="396617632"/>
+        <c:axId val="396618416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536480512"/>
+        <c:axId val="396617632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6605,7 +6612,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536486000"/>
+        <c:crossAx val="396618416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6613,7 +6620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536486000"/>
+        <c:axId val="396618416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6725,7 +6732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536480512"/>
+        <c:crossAx val="396617632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7072,11 +7079,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533647912"/>
-        <c:axId val="533193760"/>
+        <c:axId val="395141160"/>
+        <c:axId val="395139984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533647912"/>
+        <c:axId val="395141160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7086,7 +7093,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533193760"/>
+        <c:crossAx val="395139984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7094,7 +7101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533193760"/>
+        <c:axId val="395139984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7130,7 +7137,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533647912"/>
+        <c:crossAx val="395141160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7336,11 +7343,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="536486392"/>
-        <c:axId val="536488352"/>
+        <c:axId val="396618808"/>
+        <c:axId val="396619200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536486392"/>
+        <c:axId val="396618808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7438,7 +7445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536488352"/>
+        <c:crossAx val="396619200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7446,7 +7453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536488352"/>
+        <c:axId val="396619200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7553,7 +7560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536486392"/>
+        <c:crossAx val="396618808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7941,11 +7948,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536477376"/>
-        <c:axId val="536486784"/>
+        <c:axId val="395847200"/>
+        <c:axId val="395841712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536477376"/>
+        <c:axId val="395847200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8048,7 +8055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536486784"/>
+        <c:crossAx val="395841712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8056,7 +8063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536486784"/>
+        <c:axId val="395841712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8163,7 +8170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536477376"/>
+        <c:crossAx val="395847200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8258,7 +8265,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8527,11 +8533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536489136"/>
-        <c:axId val="536481688"/>
+        <c:axId val="395843672"/>
+        <c:axId val="395846808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536489136"/>
+        <c:axId val="395843672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8574,7 +8580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536481688"/>
+        <c:crossAx val="395846808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8582,7 +8588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536481688"/>
+        <c:axId val="395846808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8633,7 +8639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536489136"/>
+        <c:crossAx val="395843672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8647,7 +8653,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9019,11 +9024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536487960"/>
-        <c:axId val="536476984"/>
+        <c:axId val="395845240"/>
+        <c:axId val="395846416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536487960"/>
+        <c:axId val="395845240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9066,7 +9071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536476984"/>
+        <c:crossAx val="395846416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9074,7 +9079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536476984"/>
+        <c:axId val="395846416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9125,7 +9130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536487960"/>
+        <c:crossAx val="395845240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9470,11 +9475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536481296"/>
-        <c:axId val="536482472"/>
+        <c:axId val="395841320"/>
+        <c:axId val="395847592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536481296"/>
+        <c:axId val="395841320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9517,7 +9522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536482472"/>
+        <c:crossAx val="395847592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9525,7 +9530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536482472"/>
+        <c:axId val="395847592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9576,7 +9581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536481296"/>
+        <c:crossAx val="395841320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9952,11 +9957,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536479336"/>
-        <c:axId val="536479728"/>
+        <c:axId val="395847984"/>
+        <c:axId val="395848768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536479336"/>
+        <c:axId val="395847984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9999,7 +10004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536479728"/>
+        <c:crossAx val="395848768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10007,7 +10012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536479728"/>
+        <c:axId val="395848768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10058,7 +10063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536479336"/>
+        <c:crossAx val="395847984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10356,11 +10361,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="536483256"/>
-        <c:axId val="536483648"/>
+        <c:axId val="395848376"/>
+        <c:axId val="395844064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536483256"/>
+        <c:axId val="395848376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10402,7 +10407,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536483648"/>
+        <c:crossAx val="395844064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10410,7 +10415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536483648"/>
+        <c:axId val="395844064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10461,7 +10466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536483256"/>
+        <c:crossAx val="395848376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10871,11 +10876,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="536495800"/>
-        <c:axId val="536490312"/>
+        <c:axId val="395844848"/>
+        <c:axId val="397909104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="536495800"/>
+        <c:axId val="395844848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10978,7 +10983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536490312"/>
+        <c:crossAx val="397909104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10986,7 +10991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536490312"/>
+        <c:axId val="397909104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11092,7 +11097,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536495800"/>
+        <c:crossAx val="395844848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11437,11 +11442,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533197680"/>
-        <c:axId val="533196896"/>
+        <c:axId val="395137632"/>
+        <c:axId val="395141552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533197680"/>
+        <c:axId val="395137632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11451,7 +11456,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533196896"/>
+        <c:crossAx val="395141552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11459,7 +11464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533196896"/>
+        <c:axId val="395141552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11495,7 +11500,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533197680"/>
+        <c:crossAx val="395137632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11781,11 +11786,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533189448"/>
-        <c:axId val="533194152"/>
+        <c:axId val="395134496"/>
+        <c:axId val="395141944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533189448"/>
+        <c:axId val="395134496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11795,7 +11800,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533194152"/>
+        <c:crossAx val="395141944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11803,7 +11808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533194152"/>
+        <c:axId val="395141944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11835,7 +11840,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533189448"/>
+        <c:crossAx val="395134496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12121,11 +12126,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533188272"/>
-        <c:axId val="533188664"/>
+        <c:axId val="395140376"/>
+        <c:axId val="395140768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533188272"/>
+        <c:axId val="395140376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12135,7 +12140,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533188664"/>
+        <c:crossAx val="395140768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12143,7 +12148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533188664"/>
+        <c:axId val="395140768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12172,7 +12177,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="533188272"/>
+        <c:crossAx val="395140376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12513,11 +12518,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533194544"/>
-        <c:axId val="533191800"/>
+        <c:axId val="395668952"/>
+        <c:axId val="395671696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533194544"/>
+        <c:axId val="395668952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12560,7 +12565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533191800"/>
+        <c:crossAx val="395671696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12568,7 +12573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533191800"/>
+        <c:axId val="395671696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12619,7 +12624,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533194544"/>
+        <c:crossAx val="395668952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12802,11 +12807,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533187488"/>
-        <c:axId val="533187880"/>
+        <c:axId val="395670520"/>
+        <c:axId val="395673656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533187488"/>
+        <c:axId val="395670520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12848,7 +12853,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533187880"/>
+        <c:crossAx val="395673656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12856,7 +12861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533187880"/>
+        <c:axId val="395673656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12907,7 +12912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533187488"/>
+        <c:crossAx val="395670520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12996,6 +13001,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13059,44 +13065,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
@@ -13104,30 +13113,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$K$2:$K$13</c:f>
+              <c:f>DTemp!$K$2:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40289256198347106</c:v>
+                  <c:v>0.3732638888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7024793388429752</c:v>
+                  <c:v>0.65972222222222221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89876033057851235</c:v>
+                  <c:v>0.859375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99173553719008267</c:v>
+                  <c:v>0.97222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.99826388888888884</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -13142,6 +13151,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -13177,44 +13189,47 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
@@ -13222,44 +13237,47 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$J$2:$J$13</c:f>
+              <c:f>DTemp!$J$2:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40289256198347106</c:v>
+                  <c:v>0.2880859375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7024793388429752</c:v>
+                  <c:v>0.52734375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89876033057851235</c:v>
+                  <c:v>0.7177734375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99173553719008267</c:v>
+                  <c:v>0.859375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98140495867768596</c:v>
+                  <c:v>0.9521484375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.86776859504132231</c:v>
+                  <c:v>0.99609375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.65082644628099173</c:v>
+                  <c:v>0.96484375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33057851239669422</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.33984375</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -13276,11 +13294,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533190624"/>
-        <c:axId val="533189056"/>
+        <c:axId val="395669344"/>
+        <c:axId val="395669736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533190624"/>
+        <c:axId val="395669344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13323,7 +13341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533189056"/>
+        <c:crossAx val="395669736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13331,7 +13349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533189056"/>
+        <c:axId val="395669736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13382,7 +13400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533190624"/>
+        <c:crossAx val="395669344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13396,6 +13414,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13502,6 +13521,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13565,7 +13585,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -13610,45 +13630,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$S$2:$S$13</c:f>
+              <c:f>DTemp!$S$3:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.95407940233607225</c:v>
+                  <c:v>8.7839328137252384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.028352085993442</c:v>
+                  <c:v>15.165763909380916</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.804753817800119</c:v>
+                  <c:v>19.57295581940248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.21861625275837</c:v>
+                  <c:v>21.942004458119005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.218823121913047</c:v>
+                  <c:v>22.228771506287014</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.19307209452063</c:v>
+                  <c:v>20.500052584090543</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.495424991010037</c:v>
+                  <c:v>20.259877893779418</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.893997510158151</c:v>
+                  <c:v>17.732456485930808</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.78506404820763</c:v>
+                  <c:v>13.313969853746393</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>15.265270437377154</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>21.588352485831837</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>30.530540874754308</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43.176704971663675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13683,7 +13703,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>DTemp!$D$2:$D$13</c:f>
+              <c:f>DTemp!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -13728,45 +13748,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DTemp!$T$2:$T$13</c:f>
+              <c:f>DTemp!$T$3:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.95407940233607225</c:v>
+                  <c:v>6.9334101431274924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.028352085993442</c:v>
+                  <c:v>12.314077215533102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.804753817800119</c:v>
+                  <c:v>16.570189740526899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.21861625275837</c:v>
+                  <c:v>19.616647373343927</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.218823121913047</c:v>
+                  <c:v>21.326559912334606</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.862155037170293</c:v>
+                  <c:v>21.542786020012187</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.530097417810502</c:v>
+                  <c:v>19.737357940846241</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.36740702634836</c:v>
+                  <c:v>15.207501169120249</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.098260060792189</c:v>
+                  <c:v>11.650512352846588</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>15.265270437377154</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>21.588352485831837</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>30.530540874754308</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43.176704971663675</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13782,11 +13802,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="533192584"/>
-        <c:axId val="533189840"/>
+        <c:axId val="395674440"/>
+        <c:axId val="395667776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="533192584"/>
+        <c:axId val="395674440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13829,7 +13849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533189840"/>
+        <c:crossAx val="395667776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13837,7 +13857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="533189840"/>
+        <c:axId val="395667776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13888,7 +13908,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="533192584"/>
+        <c:crossAx val="395674440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13902,6 +13922,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26570,13 +26591,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26599,15 +26620,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26632,13 +26653,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26664,13 +26685,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -26696,13 +26717,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -27425,43 +27446,43 @@
       <selection activeCell="AI33" sqref="AI33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="6" width="9.109375" style="27"/>
+    <col min="1" max="6" width="9.140625" style="27"/>
     <col min="7" max="8" width="0" style="27" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="27"/>
-    <col min="10" max="10" width="14.44140625" style="27" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="27"/>
+    <col min="10" max="10" width="14.42578125" style="27" customWidth="1"/>
     <col min="11" max="11" width="15" style="27" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="27" customWidth="1"/>
-    <col min="13" max="13" width="19.44140625" style="27" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="27" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" style="27" customWidth="1"/>
-    <col min="16" max="16" width="19.109375" style="27" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" style="27" customWidth="1"/>
-    <col min="18" max="18" width="19.109375" style="27" customWidth="1"/>
-    <col min="19" max="20" width="13.6640625" style="27" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" style="27" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" style="27" customWidth="1"/>
-    <col min="23" max="23" width="19.44140625" style="27" customWidth="1"/>
-    <col min="24" max="24" width="21.44140625" style="27" customWidth="1"/>
-    <col min="25" max="25" width="23.33203125" style="27" customWidth="1"/>
-    <col min="26" max="26" width="20.5546875" style="27" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="27" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="27" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" style="27" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="27" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" style="27" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="27" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="27" customWidth="1"/>
+    <col min="19" max="20" width="13.7109375" style="27" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="27" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" style="27" customWidth="1"/>
+    <col min="23" max="23" width="19.42578125" style="27" customWidth="1"/>
+    <col min="24" max="24" width="21.42578125" style="27" customWidth="1"/>
+    <col min="25" max="25" width="23.28515625" style="27" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" style="27" customWidth="1"/>
     <col min="27" max="27" width="7" style="27" customWidth="1"/>
-    <col min="28" max="28" width="14.88671875" style="27" customWidth="1"/>
-    <col min="29" max="30" width="9.109375" style="27"/>
-    <col min="31" max="31" width="13.6640625" style="27" customWidth="1"/>
-    <col min="32" max="32" width="9.109375" style="27"/>
-    <col min="33" max="33" width="14.109375" style="27" customWidth="1"/>
-    <col min="34" max="34" width="10.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.109375" style="27"/>
-    <col min="36" max="36" width="16.33203125" style="27" customWidth="1"/>
-    <col min="37" max="37" width="16.88671875" style="27" customWidth="1"/>
-    <col min="38" max="43" width="9.109375" style="27"/>
-    <col min="44" max="44" width="11.6640625" style="27" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="27"/>
+    <col min="28" max="28" width="14.85546875" style="27" customWidth="1"/>
+    <col min="29" max="30" width="9.140625" style="27"/>
+    <col min="31" max="31" width="13.7109375" style="27" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" style="27"/>
+    <col min="33" max="33" width="14.140625" style="27" customWidth="1"/>
+    <col min="34" max="34" width="10.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="27"/>
+    <col min="36" max="36" width="16.28515625" style="27" customWidth="1"/>
+    <col min="37" max="37" width="16.85546875" style="27" customWidth="1"/>
+    <col min="38" max="43" width="9.140625" style="27"/>
+    <col min="44" max="44" width="11.7109375" style="27" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="15" thickBot="1">
+    <row r="1" spans="1:57" ht="15.75" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>58</v>
       </c>
@@ -28704,7 +28725,7 @@
       <c r="AH12" s="50"/>
       <c r="AI12" s="50"/>
     </row>
-    <row r="13" spans="1:57" ht="15" thickBot="1">
+    <row r="13" spans="1:57" ht="15.75" thickBot="1">
       <c r="B13" s="27">
         <v>40</v>
       </c>
@@ -28926,7 +28947,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:49" ht="15" thickBot="1">
+    <row r="19" spans="1:49" ht="15.75" thickBot="1">
       <c r="G19" s="27" t="s">
         <v>106</v>
       </c>
@@ -28962,7 +28983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:49" ht="15" thickBot="1">
+    <row r="20" spans="1:49" ht="15.75" thickBot="1">
       <c r="A20" s="27" t="s">
         <v>55</v>
       </c>
@@ -29040,7 +29061,7 @@
       <c r="AV20" s="8"/>
       <c r="AW20" s="8"/>
     </row>
-    <row r="21" spans="1:49" ht="15" thickBot="1">
+    <row r="21" spans="1:49" ht="15.75" thickBot="1">
       <c r="G21" s="11">
         <f>IF(Tday &lt;0,0.61078 * EXP(21.87456 * Tday / (Tday + 265.5)),0.61078 * EXP(17.26939 * Tday / (Tday + 237.3)))</f>
         <v>0.61077999999999999</v>
@@ -29134,7 +29155,7 @@
       <c r="AV21" s="8"/>
       <c r="AW21" s="8"/>
     </row>
-    <row r="22" spans="1:49" ht="15" thickBot="1">
+    <row r="22" spans="1:49" ht="15.75" thickBot="1">
       <c r="G22" s="11">
         <f>IF(E3 &lt;0,0.61078 * EXP(21.87456 * E3 / (E3 + 265.5)),0.61078 * EXP(17.26939 * E3 / (E3 + 237.3)))</f>
         <v>0.87227141748882542</v>
@@ -29219,7 +29240,7 @@
       <c r="AV22" s="8"/>
       <c r="AW22" s="8"/>
     </row>
-    <row r="23" spans="1:49" ht="15" thickBot="1">
+    <row r="23" spans="1:49" ht="15.75" thickBot="1">
       <c r="G23" s="11">
         <f t="shared" ref="G23:G32" si="31">IF(E4 &lt;0,0.61078 * EXP(21.87456 * E4 / (E4 + 265.5)),0.61078 * EXP(17.26939 * E4 / (E4 + 237.3)))</f>
         <v>1.2278921229539039</v>
@@ -29305,7 +29326,7 @@
       <c r="AV23" s="8"/>
       <c r="AW23" s="8"/>
     </row>
-    <row r="24" spans="1:49" ht="15" thickBot="1">
+    <row r="24" spans="1:49" ht="15.75" thickBot="1">
       <c r="G24" s="11">
         <f t="shared" si="31"/>
         <v>1.7052285488209411</v>
@@ -29394,7 +29415,7 @@
       <c r="AV24" s="8"/>
       <c r="AW24" s="8"/>
     </row>
-    <row r="25" spans="1:49" ht="15" thickBot="1">
+    <row r="25" spans="1:49" ht="15.75" thickBot="1">
       <c r="G25" s="11">
         <f t="shared" si="31"/>
         <v>2.3380938419374377</v>
@@ -29487,7 +29508,7 @@
       <c r="AV25" s="8"/>
       <c r="AW25" s="8"/>
     </row>
-    <row r="26" spans="1:49" ht="15" thickBot="1">
+    <row r="26" spans="1:49" ht="15.75" thickBot="1">
       <c r="G26" s="11">
         <f t="shared" si="31"/>
         <v>3.1674898302368564</v>
@@ -29579,7 +29600,7 @@
       <c r="AV26" s="8"/>
       <c r="AW26" s="8"/>
     </row>
-    <row r="27" spans="1:49" ht="15" thickBot="1">
+    <row r="27" spans="1:49" ht="15.75" thickBot="1">
       <c r="G27" s="11">
         <f t="shared" si="31"/>
         <v>4.2426356531114431</v>
@@ -29663,7 +29684,7 @@
       <c r="AV27" s="8"/>
       <c r="AW27" s="8"/>
     </row>
-    <row r="28" spans="1:49" ht="15" thickBot="1">
+    <row r="28" spans="1:49" ht="15.75" thickBot="1">
       <c r="G28" s="11">
         <f t="shared" si="31"/>
         <v>5.6220563085635584</v>
@@ -29747,7 +29768,7 @@
       <c r="AV28" s="8"/>
       <c r="AW28" s="8"/>
     </row>
-    <row r="29" spans="1:49" ht="15" thickBot="1">
+    <row r="29" spans="1:49" ht="15.75" thickBot="1">
       <c r="G29" s="11">
         <f t="shared" si="31"/>
         <v>7.3747231460360023</v>
@@ -29833,7 +29854,7 @@
       <c r="AV29" s="8"/>
       <c r="AW29" s="8"/>
     </row>
-    <row r="30" spans="1:49" ht="15" thickBot="1">
+    <row r="30" spans="1:49" ht="15.75" thickBot="1">
       <c r="G30" s="11">
         <f t="shared" si="31"/>
         <v>9.5812372781996284</v>
@@ -29929,7 +29950,7 @@
       <c r="AV30" s="8"/>
       <c r="AW30" s="8"/>
     </row>
-    <row r="31" spans="1:49" ht="15" thickBot="1">
+    <row r="31" spans="1:49" ht="15.75" thickBot="1">
       <c r="G31" s="11">
         <f t="shared" si="31"/>
         <v>12.335046017492973</v>
@@ -30018,7 +30039,7 @@
       <c r="AV31" s="8"/>
       <c r="AW31" s="8"/>
     </row>
-    <row r="32" spans="1:49" ht="15" thickBot="1">
+    <row r="32" spans="1:49" ht="15.75" thickBot="1">
       <c r="G32" s="12">
         <f t="shared" si="31"/>
         <v>15.743681776119971</v>
@@ -30704,14 +30725,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="27"/>
-    <col min="2" max="2" width="12.44140625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="27"/>
-    <col min="5" max="5" width="12.33203125" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="27"/>
+    <col min="1" max="1" width="9.140625" style="27"/>
+    <col min="2" max="2" width="12.42578125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="27"/>
+    <col min="5" max="5" width="12.28515625" style="27" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -30752,7 +30773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="27">
         <v>20</v>
       </c>
@@ -31049,7 +31070,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -31134,22 +31155,22 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AC18"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="6" max="7" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="27"/>
-    <col min="14" max="14" width="9.109375" style="27"/>
-    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="27"/>
+    <col min="14" max="14" width="9.140625" style="27"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -31226,57 +31247,64 @@
         <v>1</v>
       </c>
       <c r="AA1" s="31">
+        <v>-5</v>
+      </c>
+      <c r="AB1" s="29">
+        <f>AA2+(AA2-AA3)</f>
+        <v>11</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" s="27" customFormat="1">
+      <c r="A2" s="27">
+        <v>-20</v>
+      </c>
+      <c r="B2" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2">
-        <v>-15</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
+      <c r="C2" s="27">
         <f>(A2+B2)/2</f>
+        <v>-10</v>
+      </c>
+      <c r="D2" s="27">
+        <f>(C2+B2)/2</f>
         <v>-5</v>
       </c>
-      <c r="D2">
-        <f>(C2+B2)/2</f>
+      <c r="E2" s="27">
+        <f>(C2+ AA$2)/2</f>
+        <v>8.5</v>
+      </c>
+      <c r="F2" s="27">
+        <f>0.61078 * EXP(17.26939 * D2 / (D2 + 237.3))</f>
+        <v>0.42116823077156701</v>
+      </c>
+      <c r="G2" s="27">
+        <f>0.61078 * EXP(17.26939 * A2 / (A2 + 237.3))</f>
+        <v>0.12462202785072264</v>
+      </c>
+      <c r="H2" s="27">
+        <f>F2-G2</f>
+        <v>0.29654620292084438</v>
+      </c>
+      <c r="I2" s="27">
+        <f>MAX(0, 1 - AA$8 * H2^ AA$9)</f>
+        <v>0.99560301747666147</v>
+      </c>
+      <c r="J2" s="27">
+        <f>IF(D2&lt;=$AA$2,MAX(0,(($AB$3-D2)*(D2-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D2)*(D2-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
         <v>0</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E13" si="0">(C2+ AA$2)/2</f>
-        <v>8.5</v>
-      </c>
-      <c r="F2">
-        <f>0.61078 * EXP(17.26939 * D2 / (D2 + 237.3))</f>
-        <v>0.61077999999999999</v>
-      </c>
-      <c r="G2">
-        <f>0.61078 * EXP(17.26939 * A2 / (A2 + 237.3))</f>
-        <v>0.19046355243449331</v>
-      </c>
-      <c r="H2">
-        <f>F2-G2</f>
-        <v>0.42031644756550668</v>
-      </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I13" si="1">MAX(0, 1 - AA$8 * H2^ AA$9)</f>
-        <v>0.99116670419529562</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J13" si="2">MAX(0,(($AA$3-D2)*(D2-$AA$1))/((($AA$3-$AA$1)/2)^2))</f>
+      <c r="K2" s="27">
+        <f>IF(D2&gt;AA$2,1,MAX(0,((AA$3-D2)*(D2-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
         <v>0</v>
       </c>
-      <c r="K2" s="27">
-        <f t="shared" ref="K2:K13" si="3">IF(D2&gt;AA$2,1,MAX(0,((AA$3-D2)*(D2-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L13" si="4">AA$10*(AA$7*I2*AA$11*12)/1000000000</f>
-        <v>2.1725371888189602</v>
-      </c>
-      <c r="M2">
+      <c r="L2" s="27">
+        <f>AA$10*(AA$7*I2*AA$11*12)/1000000000</f>
+        <v>2.182261138931715</v>
+      </c>
+      <c r="M2" s="27">
         <f>K2*L2</f>
         <v>0</v>
       </c>
@@ -31285,249 +31313,258 @@
         <v>0</v>
       </c>
       <c r="O2" s="27">
-        <f t="shared" ref="O2:O13" si="5" xml:space="preserve"> AA$12*AA$13* M2 * AA$14</f>
+        <f xml:space="preserve"> AA$12*AA$13* M2 * AA$14</f>
         <v>0</v>
       </c>
       <c r="P2" s="27">
-        <f t="shared" ref="P2:P13" si="6" xml:space="preserve"> AA$12*AA$13* N2 * AA$14</f>
+        <f xml:space="preserve"> AA$12*AA$13* N2 * AA$14</f>
         <v>0</v>
       </c>
-      <c r="Q2">
-        <f t="shared" ref="Q2:Q13" si="7">AA$18^((D2-AA$2)/10)</f>
-        <v>0.21763764082403106</v>
-      </c>
-      <c r="R2">
-        <f t="shared" ref="R2:R13" si="8">AA$17*Q2</f>
-        <v>2.1763764082403107E-2</v>
-      </c>
-      <c r="S2">
+      <c r="Q2" s="27">
+        <f>AA$18^((D2-AA$2)/10)</f>
+        <v>0.10881882041201553</v>
+      </c>
+      <c r="R2" s="27">
+        <f>AA$17*Q2</f>
+        <v>1.0881882041201553E-2</v>
+      </c>
+      <c r="S2" s="27">
         <f>O2+V2</f>
-        <v>0.95407940233607225</v>
+        <v>0.47703970116803612</v>
       </c>
       <c r="T2" s="27">
         <f>P2+V2</f>
-        <v>0.95407940233607225</v>
-      </c>
-      <c r="U2">
+        <v>0.47703970116803612</v>
+      </c>
+      <c r="U2" s="27">
         <f>AA$17*Q2*AA$10*86400*12/1000000000*AA$7</f>
-        <v>9.5407940233607227E-2</v>
-      </c>
-      <c r="V2">
+        <v>4.7703970116803614E-2</v>
+      </c>
+      <c r="V2" s="27">
         <f>AA$12*U2*AA$14</f>
-        <v>0.95407940233607225</v>
-      </c>
-      <c r="W2">
-        <f t="shared" ref="W2:W13" si="9">AA$16/H2</f>
-        <v>25.932841941192954</v>
-      </c>
-      <c r="X2">
-        <f t="shared" ref="X2:X13" si="10">T2*(44/12)/W2</f>
-        <v>0.13489810140484756</v>
+        <v>0.47703970116803612</v>
+      </c>
+      <c r="W2" s="27">
+        <f>AA$16/H2</f>
+        <v>36.756498288091329</v>
+      </c>
+      <c r="X2" s="27">
+        <f t="shared" ref="X2" si="0">T2*(44/12)/W2</f>
+        <v>4.7587383249621688E-2</v>
       </c>
       <c r="Z2" s="31" t="s">
         <v>2</v>
       </c>
       <c r="AA2" s="31">
-        <v>22</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:30">
       <c r="A3">
-        <v>-10</v>
+        <v>-15</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="11">(A3+B3)/2</f>
+        <f>(A3+B3)/2</f>
+        <v>-5</v>
+      </c>
+      <c r="D3">
+        <f>(C3+B3)/2</f>
         <v>0</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D13" si="12">(C3+B3)/2</f>
-        <v>5</v>
-      </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f>(C3+ AA$2)/2</f>
         <v>11</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F13" si="13">0.61078 * EXP(17.26939 * D3 / (D3 + 237.3))</f>
-        <v>0.87227141748882542</v>
+        <f>0.61078 * EXP(17.26939 * D3 / (D3 + 237.3))</f>
+        <v>0.61077999999999999</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G13" si="14">0.61078 * EXP(17.26939 * A3 / (A3 + 237.3))</f>
-        <v>0.28570929427727804</v>
+        <f>0.61078 * EXP(17.26939 * A3 / (A3 + 237.3))</f>
+        <v>0.19046355243449331</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H13" si="15">F3-G3</f>
-        <v>0.58656212321154744</v>
+        <f>F3-G3</f>
+        <v>0.42031644756550668</v>
       </c>
       <c r="I3">
-        <f t="shared" si="1"/>
-        <v>0.98279724378067812</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="2"/>
-        <v>0.40289256198347106</v>
+        <f>MAX(0, 1 - AA$8 * H3^ AA$9)</f>
+        <v>0.99116670419529562</v>
+      </c>
+      <c r="J3" s="27">
+        <f>IF(D3&lt;=$AA$2,MAX(0,(($AB$3-D3)*(D3-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D3)*(D3-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.2880859375</v>
       </c>
       <c r="K3" s="27">
-        <f t="shared" si="3"/>
-        <v>0.40289256198347106</v>
-      </c>
-      <c r="L3" s="27">
-        <f t="shared" si="4"/>
-        <v>2.1541921779099553</v>
-      </c>
-      <c r="M3" s="27">
-        <f t="shared" ref="M3:M13" si="16">K3*L3</f>
-        <v>0.86790800556289516</v>
+        <f>IF(D3&gt;AA$2,1,MAX(0,((AA$3-D3)*(D3-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>0.3732638888888889</v>
+      </c>
+      <c r="L3">
+        <f>AA$10*(AA$7*I3*AA$11*12)/1000000000</f>
+        <v>2.1725371888189602</v>
+      </c>
+      <c r="M3">
+        <f>K3*L3</f>
+        <v>0.81092967985429942</v>
       </c>
       <c r="N3" s="27">
-        <f t="shared" ref="N3:N13" si="17">J3*L3</f>
-        <v>0.86790800556289516</v>
+        <f>J3*L3</f>
+        <v>0.62587741279452469</v>
       </c>
       <c r="O3" s="27">
-        <f t="shared" si="5"/>
-        <v>8.6790800556289511</v>
+        <f xml:space="preserve"> AA$12*AA$13* M3 * AA$14</f>
+        <v>8.109296798542994</v>
       </c>
       <c r="P3" s="27">
-        <f t="shared" si="6"/>
-        <v>8.6790800556289511</v>
-      </c>
-      <c r="Q3" s="27">
-        <f t="shared" si="7"/>
-        <v>0.30778610333622908</v>
-      </c>
-      <c r="R3" s="27">
-        <f t="shared" si="8"/>
-        <v>3.0778610333622908E-2</v>
-      </c>
-      <c r="S3" s="27">
-        <f t="shared" ref="S3:S13" si="18">O3+V3</f>
-        <v>10.028352085993442</v>
+        <f xml:space="preserve"> AA$12*AA$13* N3 * AA$14</f>
+        <v>6.2587741279452471</v>
+      </c>
+      <c r="Q3">
+        <f>AA$18^((D3-AA$2)/10)</f>
+        <v>0.15389305166811451</v>
+      </c>
+      <c r="R3">
+        <f>AA$17*Q3</f>
+        <v>1.5389305166811452E-2</v>
+      </c>
+      <c r="S3">
+        <f>O3+V3</f>
+        <v>8.7839328137252384</v>
       </c>
       <c r="T3" s="27">
-        <f t="shared" ref="T3:T13" si="19">P3+V3</f>
-        <v>10.028352085993442</v>
-      </c>
-      <c r="U3" s="27">
-        <f t="shared" ref="U3:U13" si="20">AA$17*Q3*AA$10*86400*12/1000000000*AA$7</f>
-        <v>0.13492720303644898</v>
-      </c>
-      <c r="V3" s="27">
-        <f t="shared" ref="V3:V13" si="21">AA$12*U3*AA$14</f>
-        <v>1.3492720303644898</v>
+        <f>P3+V3</f>
+        <v>6.9334101431274924</v>
+      </c>
+      <c r="U3">
+        <f>AA$17*Q3*AA$10*86400*12/1000000000*AA$7</f>
+        <v>6.7463601518224489E-2</v>
+      </c>
+      <c r="V3">
+        <f>AA$12*U3*AA$14</f>
+        <v>0.67463601518224492</v>
       </c>
       <c r="W3">
-        <f t="shared" si="9"/>
-        <v>18.582856902386187</v>
+        <f>AA$16/H3</f>
+        <v>25.932841941192954</v>
       </c>
       <c r="X3">
-        <f t="shared" si="10"/>
-        <v>1.9787390339634829</v>
+        <f t="shared" ref="X3:X14" si="1">T3*(44/12)/W3</f>
+        <v>0.98032078072214024</v>
       </c>
       <c r="Z3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="AA3" s="29">
+      <c r="AA3" s="31">
+        <v>43</v>
+      </c>
+      <c r="AB3" s="29">
         <f>AA2+(AA2-AA1)</f>
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:30">
       <c r="A4">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="C4:C11" si="2">(A4+B4)/2</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D14" si="3">(C4+B4)/2</f>
         <v>5</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>(C4+ AA$2)/2</f>
         <v>13.5</v>
       </c>
       <c r="F4">
-        <f t="shared" si="13"/>
-        <v>1.2278921229539039</v>
+        <f t="shared" ref="F4:F14" si="4">0.61078 * EXP(17.26939 * D4 / (D4 + 237.3))</f>
+        <v>0.87227141748882542</v>
       </c>
       <c r="G4">
-        <f t="shared" si="14"/>
-        <v>0.42116823077156701</v>
+        <f t="shared" ref="G4:G14" si="5">0.61078 * EXP(17.26939 * A4 / (A4 + 237.3))</f>
+        <v>0.28570929427727804</v>
       </c>
       <c r="H4">
-        <f t="shared" si="15"/>
-        <v>0.80672389218233698</v>
+        <f t="shared" ref="H4:H14" si="6">F4-G4</f>
+        <v>0.58656212321154744</v>
       </c>
       <c r="I4">
+        <f>MAX(0, 1 - AA$8 * H4^ AA$9)</f>
+        <v>0.98279724378067812</v>
+      </c>
+      <c r="J4" s="27">
+        <f>IF(D4&lt;=$AA$2,MAX(0,(($AB$3-D4)*(D4-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D4)*(D4-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.52734375</v>
+      </c>
+      <c r="K4" s="27">
+        <f>IF(D4&gt;AA$2,1,MAX(0,((AA$3-D4)*(D4-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="L4" s="27">
+        <f>AA$10*(AA$7*I4*AA$11*12)/1000000000</f>
+        <v>2.1541921779099553</v>
+      </c>
+      <c r="M4" s="27">
+        <f t="shared" ref="M4:M14" si="7">K4*L4</f>
+        <v>1.4211684507044844</v>
+      </c>
+      <c r="N4" s="27">
+        <f t="shared" ref="N4:N14" si="8">J4*L4</f>
+        <v>1.1359997813197029</v>
+      </c>
+      <c r="O4" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M4 * AA$14</f>
+        <v>14.211684507044843</v>
+      </c>
+      <c r="P4" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N4 * AA$14</f>
+        <v>11.35999781319703</v>
+      </c>
+      <c r="Q4" s="27">
+        <f>AA$18^((D4-AA$2)/10)</f>
+        <v>0.21763764082403106</v>
+      </c>
+      <c r="R4" s="27">
+        <f>AA$17*Q4</f>
+        <v>2.1763764082403107E-2</v>
+      </c>
+      <c r="S4" s="27">
+        <f t="shared" ref="S4:S14" si="9">O4+V4</f>
+        <v>15.165763909380916</v>
+      </c>
+      <c r="T4" s="27">
+        <f t="shared" ref="T4:T14" si="10">P4+V4</f>
+        <v>12.314077215533102</v>
+      </c>
+      <c r="U4" s="27">
+        <f>AA$17*Q4*AA$10*86400*12/1000000000*AA$7</f>
+        <v>9.5407940233607227E-2</v>
+      </c>
+      <c r="V4" s="27">
+        <f>AA$12*U4*AA$14</f>
+        <v>0.95407940233607225</v>
+      </c>
+      <c r="W4">
+        <f>AA$16/H4</f>
+        <v>18.582856902386187</v>
+      </c>
+      <c r="X4">
         <f t="shared" si="1"/>
-        <v>0.96745982808910902</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>0.7024793388429752</v>
-      </c>
-      <c r="K4" s="27">
-        <f t="shared" si="3"/>
-        <v>0.7024793388429752</v>
-      </c>
-      <c r="L4" s="27">
-        <f t="shared" si="4"/>
-        <v>2.1205741136335114</v>
-      </c>
-      <c r="M4" s="27">
-        <f t="shared" si="16"/>
-        <v>1.4896595013127973</v>
-      </c>
-      <c r="N4" s="27">
-        <f t="shared" si="17"/>
-        <v>1.4896595013127973</v>
-      </c>
-      <c r="O4" s="27">
-        <f t="shared" si="5"/>
-        <v>14.896595013127973</v>
-      </c>
-      <c r="P4" s="27">
-        <f t="shared" si="6"/>
-        <v>14.896595013127973</v>
-      </c>
-      <c r="Q4" s="27">
-        <f t="shared" si="7"/>
-        <v>0.43527528164806206</v>
-      </c>
-      <c r="R4" s="27">
-        <f t="shared" si="8"/>
-        <v>4.3527528164806206E-2</v>
-      </c>
-      <c r="S4" s="27">
-        <f t="shared" si="18"/>
-        <v>16.804753817800119</v>
-      </c>
-      <c r="T4" s="27">
-        <f t="shared" si="19"/>
-        <v>16.804753817800119</v>
-      </c>
-      <c r="U4" s="27">
-        <f t="shared" si="20"/>
-        <v>0.19081588046721443</v>
-      </c>
-      <c r="V4" s="27">
-        <f t="shared" si="21"/>
-        <v>1.9081588046721443</v>
-      </c>
-      <c r="W4">
-        <f t="shared" si="9"/>
-        <v>13.511438183036192</v>
-      </c>
-      <c r="X4">
-        <f t="shared" si="10"/>
-        <v>4.560390228675189</v>
+        <v>2.4297456894885134</v>
       </c>
       <c r="Z4" s="31" t="s">
         <v>6</v>
@@ -31536,100 +31573,100 @@
         <v>-46</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:30">
       <c r="A5">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="12"/>
-        <v>15</v>
-      </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>(C5+ AA$2)/2</f>
         <v>16</v>
       </c>
       <c r="F5">
-        <f t="shared" si="13"/>
-        <v>1.7052285488209411</v>
+        <f t="shared" si="4"/>
+        <v>1.2278921229539039</v>
       </c>
       <c r="G5">
-        <f t="shared" si="14"/>
-        <v>0.61077999999999999</v>
+        <f t="shared" si="5"/>
+        <v>0.42116823077156701</v>
       </c>
       <c r="H5">
-        <f t="shared" si="15"/>
-        <v>1.094448548820941</v>
+        <f t="shared" si="6"/>
+        <v>0.80672389218233698</v>
       </c>
       <c r="I5">
+        <f>MAX(0, 1 - AA$8 * H5^ AA$9)</f>
+        <v>0.96745982808910902</v>
+      </c>
+      <c r="J5" s="27">
+        <f>IF(D5&lt;=$AA$2,MAX(0,(($AB$3-D5)*(D5-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D5)*(D5-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.7177734375</v>
+      </c>
+      <c r="K5" s="27">
+        <f>IF(D5&gt;AA$2,1,MAX(0,((AA$3-D5)*(D5-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>0.859375</v>
+      </c>
+      <c r="L5" s="27">
+        <f>AA$10*(AA$7*I5*AA$11*12)/1000000000</f>
+        <v>2.1205741136335114</v>
+      </c>
+      <c r="M5" s="27">
+        <f t="shared" si="7"/>
+        <v>1.822368378903799</v>
+      </c>
+      <c r="N5" s="27">
+        <f t="shared" si="8"/>
+        <v>1.5220917710162412</v>
+      </c>
+      <c r="O5" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M5 * AA$14</f>
+        <v>18.223683789037992</v>
+      </c>
+      <c r="P5" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N5 * AA$14</f>
+        <v>15.220917710162411</v>
+      </c>
+      <c r="Q5" s="27">
+        <f>AA$18^((D5-AA$2)/10)</f>
+        <v>0.30778610333622908</v>
+      </c>
+      <c r="R5" s="27">
+        <f>AA$17*Q5</f>
+        <v>3.0778610333622908E-2</v>
+      </c>
+      <c r="S5" s="27">
+        <f t="shared" si="9"/>
+        <v>19.57295581940248</v>
+      </c>
+      <c r="T5" s="27">
+        <f t="shared" si="10"/>
+        <v>16.570189740526899</v>
+      </c>
+      <c r="U5" s="27">
+        <f>AA$17*Q5*AA$10*86400*12/1000000000*AA$7</f>
+        <v>0.13492720303644898</v>
+      </c>
+      <c r="V5" s="27">
+        <f>AA$12*U5*AA$14</f>
+        <v>1.3492720303644898</v>
+      </c>
+      <c r="W5">
+        <f>AA$16/H5</f>
+        <v>13.511438183036192</v>
+      </c>
+      <c r="X5">
         <f t="shared" si="1"/>
-        <v>0.94010911869918679</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0.89876033057851235</v>
-      </c>
-      <c r="K5" s="27">
-        <f t="shared" si="3"/>
-        <v>0.89876033057851235</v>
-      </c>
-      <c r="L5" s="27">
-        <f t="shared" si="4"/>
-        <v>2.0606241243545345</v>
-      </c>
-      <c r="M5" s="27">
-        <f t="shared" si="16"/>
-        <v>1.8520072192029389</v>
-      </c>
-      <c r="N5" s="27">
-        <f t="shared" si="17"/>
-        <v>1.8520072192029389</v>
-      </c>
-      <c r="O5" s="27">
-        <f t="shared" si="5"/>
-        <v>18.520072192029389</v>
-      </c>
-      <c r="P5" s="27">
-        <f t="shared" si="6"/>
-        <v>18.520072192029389</v>
-      </c>
-      <c r="Q5" s="27">
-        <f t="shared" si="7"/>
-        <v>0.61557220667245816</v>
-      </c>
-      <c r="R5" s="27">
-        <f t="shared" si="8"/>
-        <v>6.1557220667245817E-2</v>
-      </c>
-      <c r="S5" s="27">
-        <f t="shared" si="18"/>
-        <v>21.21861625275837</v>
-      </c>
-      <c r="T5" s="27">
-        <f t="shared" si="19"/>
-        <v>21.21861625275837</v>
-      </c>
-      <c r="U5" s="27">
-        <f t="shared" si="20"/>
-        <v>0.26985440607289796</v>
-      </c>
-      <c r="V5" s="27">
-        <f t="shared" si="21"/>
-        <v>2.6985440607289797</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="9"/>
-        <v>9.9593535134590532</v>
-      </c>
-      <c r="X5">
-        <f t="shared" si="10"/>
-        <v>7.8119119701534592</v>
+        <v>4.4967353999527386</v>
       </c>
       <c r="Z5" s="31" t="s">
         <v>7</v>
@@ -31638,100 +31675,100 @@
         <v>71.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:30">
       <c r="A6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>(C6+ AA$2)/2</f>
         <v>18.5</v>
       </c>
       <c r="F6">
-        <f t="shared" si="13"/>
-        <v>2.3380938419374377</v>
+        <f t="shared" si="4"/>
+        <v>1.7052285488209411</v>
       </c>
       <c r="G6">
-        <f t="shared" si="14"/>
-        <v>0.87227141748882542</v>
+        <f t="shared" si="5"/>
+        <v>0.61077999999999999</v>
       </c>
       <c r="H6">
-        <f t="shared" si="15"/>
-        <v>1.4658224244486124</v>
+        <f t="shared" si="6"/>
+        <v>1.094448548820941</v>
       </c>
       <c r="I6">
+        <f>MAX(0, 1 - AA$8 * H6^ AA$9)</f>
+        <v>0.94010911869918679</v>
+      </c>
+      <c r="J6" s="27">
+        <f>IF(D6&lt;=$AA$2,MAX(0,(($AB$3-D6)*(D6-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D6)*(D6-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.859375</v>
+      </c>
+      <c r="K6" s="27">
+        <f>IF(D6&gt;AA$2,1,MAX(0,((AA$3-D6)*(D6-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="L6" s="27">
+        <f>AA$10*(AA$7*I6*AA$11*12)/1000000000</f>
+        <v>2.0606241243545345</v>
+      </c>
+      <c r="M6" s="27">
+        <f t="shared" si="7"/>
+        <v>2.0033845653446862</v>
+      </c>
+      <c r="N6" s="27">
+        <f t="shared" si="8"/>
+        <v>1.7708488568671781</v>
+      </c>
+      <c r="O6" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M6 * AA$14</f>
+        <v>20.033845653446861</v>
+      </c>
+      <c r="P6" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N6 * AA$14</f>
+        <v>17.708488568671783</v>
+      </c>
+      <c r="Q6" s="27">
+        <f>AA$18^((D6-AA$2)/10)</f>
+        <v>0.43527528164806206</v>
+      </c>
+      <c r="R6" s="27">
+        <f>AA$17*Q6</f>
+        <v>4.3527528164806206E-2</v>
+      </c>
+      <c r="S6" s="27">
+        <f t="shared" si="9"/>
+        <v>21.942004458119005</v>
+      </c>
+      <c r="T6" s="27">
+        <f t="shared" si="10"/>
+        <v>19.616647373343927</v>
+      </c>
+      <c r="U6" s="27">
+        <f>AA$17*Q6*AA$10*86400*12/1000000000*AA$7</f>
+        <v>0.19081588046721443</v>
+      </c>
+      <c r="V6" s="27">
+        <f>AA$12*U6*AA$14</f>
+        <v>1.9081588046721443</v>
+      </c>
+      <c r="W6">
+        <f>AA$16/H6</f>
+        <v>9.9593535134590532</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="1"/>
-        <v>0.89256823099917959</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>0.99173553719008267</v>
-      </c>
-      <c r="K6" s="27">
-        <f t="shared" si="3"/>
-        <v>0.99173553719008267</v>
-      </c>
-      <c r="L6" s="27">
-        <f t="shared" si="4"/>
-        <v>1.9564193058506831</v>
-      </c>
-      <c r="M6" s="27">
-        <f t="shared" si="16"/>
-        <v>1.940250551256876</v>
-      </c>
-      <c r="N6" s="27">
-        <f t="shared" si="17"/>
-        <v>1.940250551256876</v>
-      </c>
-      <c r="O6" s="27">
-        <f t="shared" si="5"/>
-        <v>19.402505512568759</v>
-      </c>
-      <c r="P6" s="27">
-        <f t="shared" si="6"/>
-        <v>19.402505512568759</v>
-      </c>
-      <c r="Q6" s="27">
-        <f t="shared" si="7"/>
-        <v>0.87055056329612412</v>
-      </c>
-      <c r="R6" s="27">
-        <f t="shared" si="8"/>
-        <v>8.7055056329612412E-2</v>
-      </c>
-      <c r="S6" s="27">
-        <f t="shared" si="18"/>
-        <v>23.218823121913047</v>
-      </c>
-      <c r="T6" s="27">
-        <f t="shared" si="19"/>
-        <v>23.218823121913047</v>
-      </c>
-      <c r="U6" s="27">
-        <f t="shared" si="20"/>
-        <v>0.38163176093442885</v>
-      </c>
-      <c r="V6" s="27">
-        <f t="shared" si="21"/>
-        <v>3.8163176093442885</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="9"/>
-        <v>7.4360985465890748</v>
-      </c>
-      <c r="X6">
-        <f t="shared" si="10"/>
-        <v>11.44897209833232</v>
+        <v>7.2221261087269788</v>
       </c>
       <c r="Z6" s="31" t="s">
         <v>8</v>
@@ -31740,100 +31777,100 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:30">
       <c r="A7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="12"/>
-        <v>25</v>
-      </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f>(C7+ AA$2)/2</f>
         <v>21</v>
       </c>
       <c r="F7">
-        <f t="shared" si="13"/>
-        <v>3.1674898302368564</v>
+        <f t="shared" si="4"/>
+        <v>2.3380938419374377</v>
       </c>
       <c r="G7">
-        <f t="shared" si="14"/>
-        <v>1.2278921229539039</v>
+        <f t="shared" si="5"/>
+        <v>0.87227141748882542</v>
       </c>
       <c r="H7">
-        <f t="shared" si="15"/>
-        <v>1.9395977072829524</v>
+        <f t="shared" si="6"/>
+        <v>1.4658224244486124</v>
       </c>
       <c r="I7">
+        <f>MAX(0, 1 - AA$8 * H7^ AA$9)</f>
+        <v>0.89256823099917959</v>
+      </c>
+      <c r="J7" s="27">
+        <f>IF(D7&lt;=$AA$2,MAX(0,(($AB$3-D7)*(D7-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D7)*(D7-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.9521484375</v>
+      </c>
+      <c r="K7" s="27">
+        <f>IF(D7&gt;AA$2,1,MAX(0,((AA$3-D7)*(D7-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>0.99826388888888884</v>
+      </c>
+      <c r="L7" s="27">
+        <f>AA$10*(AA$7*I7*AA$11*12)/1000000000</f>
+        <v>1.9564193058506831</v>
+      </c>
+      <c r="M7" s="27">
+        <f t="shared" si="7"/>
+        <v>1.9530227445558033</v>
+      </c>
+      <c r="N7" s="27">
+        <f t="shared" si="8"/>
+        <v>1.8628015851605626</v>
+      </c>
+      <c r="O7" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M7 * AA$14</f>
+        <v>19.530227445558033</v>
+      </c>
+      <c r="P7" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N7 * AA$14</f>
+        <v>18.628015851605625</v>
+      </c>
+      <c r="Q7" s="27">
+        <f>AA$18^((D7-AA$2)/10)</f>
+        <v>0.61557220667245816</v>
+      </c>
+      <c r="R7" s="27">
+        <f>AA$17*Q7</f>
+        <v>6.1557220667245817E-2</v>
+      </c>
+      <c r="S7" s="27">
+        <f t="shared" si="9"/>
+        <v>22.228771506287014</v>
+      </c>
+      <c r="T7" s="27">
+        <f t="shared" si="10"/>
+        <v>21.326559912334606</v>
+      </c>
+      <c r="U7" s="27">
+        <f>AA$17*Q7*AA$10*86400*12/1000000000*AA$7</f>
+        <v>0.26985440607289796</v>
+      </c>
+      <c r="V7" s="27">
+        <f>AA$12*U7*AA$14</f>
+        <v>2.6985440607289797</v>
+      </c>
+      <c r="W7">
+        <f>AA$16/H7</f>
+        <v>7.4360985465890748</v>
+      </c>
+      <c r="X7">
         <f t="shared" si="1"/>
-        <v>0.81189803669513572</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0.98140495867768596</v>
-      </c>
-      <c r="K7" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L7" s="27">
-        <f t="shared" si="4"/>
-        <v>1.7795983973062672</v>
-      </c>
-      <c r="M7" s="27">
-        <f t="shared" si="16"/>
-        <v>1.7795983973062672</v>
-      </c>
-      <c r="N7" s="27">
-        <f t="shared" si="17"/>
-        <v>1.7465066915712333</v>
-      </c>
-      <c r="O7" s="27">
-        <f t="shared" si="5"/>
-        <v>17.795983973062672</v>
-      </c>
-      <c r="P7" s="27">
-        <f t="shared" si="6"/>
-        <v>17.465066915712335</v>
-      </c>
-      <c r="Q7" s="27">
-        <f t="shared" si="7"/>
-        <v>1.2311444133449163</v>
-      </c>
-      <c r="R7" s="27">
-        <f t="shared" si="8"/>
-        <v>0.12311444133449163</v>
-      </c>
-      <c r="S7" s="27">
-        <f t="shared" si="18"/>
-        <v>23.19307209452063</v>
-      </c>
-      <c r="T7" s="27">
-        <f t="shared" si="19"/>
-        <v>22.862155037170293</v>
-      </c>
-      <c r="U7" s="27">
-        <f t="shared" si="20"/>
-        <v>0.53970881214579591</v>
-      </c>
-      <c r="V7" s="27">
-        <f t="shared" si="21"/>
-        <v>5.3970881214579594</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="9"/>
-        <v>5.6197220480679224</v>
-      </c>
-      <c r="X7">
-        <f t="shared" si="10"/>
-        <v>14.91673450856489</v>
+        <v>10.51591582000966</v>
       </c>
       <c r="Z7" s="31" t="s">
         <v>5</v>
@@ -31843,100 +31880,100 @@
         <v>140.94000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:30">
       <c r="A8">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="12"/>
-        <v>30</v>
-      </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f>(C8+ AA$2)/2</f>
         <v>23.5</v>
       </c>
       <c r="F8">
-        <f t="shared" si="13"/>
-        <v>4.2426356531114431</v>
+        <f t="shared" si="4"/>
+        <v>3.1674898302368564</v>
       </c>
       <c r="G8">
-        <f t="shared" si="14"/>
-        <v>1.7052285488209411</v>
+        <f t="shared" si="5"/>
+        <v>1.2278921229539039</v>
       </c>
       <c r="H8">
-        <f t="shared" si="15"/>
-        <v>2.537407104290502</v>
+        <f t="shared" si="6"/>
+        <v>1.9395977072829524</v>
       </c>
       <c r="I8">
+        <f>MAX(0, 1 - AA$8 * H8^ AA$9)</f>
+        <v>0.81189803669513572</v>
+      </c>
+      <c r="J8" s="27">
+        <f>IF(D8&lt;=$AA$2,MAX(0,(($AB$3-D8)*(D8-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D8)*(D8-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.99609375</v>
+      </c>
+      <c r="K8" s="27">
+        <f>IF(D8&gt;AA$2,1,MAX(0,((AA$3-D8)*(D8-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>0.9375</v>
+      </c>
+      <c r="L8" s="27">
+        <f>AA$10*(AA$7*I8*AA$11*12)/1000000000</f>
+        <v>1.7795983973062672</v>
+      </c>
+      <c r="M8" s="27">
+        <f t="shared" si="7"/>
+        <v>1.6683734974746256</v>
+      </c>
+      <c r="N8" s="27">
+        <f t="shared" si="8"/>
+        <v>1.7726468410667897</v>
+      </c>
+      <c r="O8" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M8 * AA$14</f>
+        <v>16.683734974746255</v>
+      </c>
+      <c r="P8" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N8 * AA$14</f>
+        <v>17.726468410667898</v>
+      </c>
+      <c r="Q8" s="27">
+        <f>AA$18^((D8-AA$2)/10)</f>
+        <v>0.87055056329612412</v>
+      </c>
+      <c r="R8" s="27">
+        <f>AA$17*Q8</f>
+        <v>8.7055056329612412E-2</v>
+      </c>
+      <c r="S8" s="27">
+        <f t="shared" si="9"/>
+        <v>20.500052584090543</v>
+      </c>
+      <c r="T8" s="27">
+        <f t="shared" si="10"/>
+        <v>21.542786020012187</v>
+      </c>
+      <c r="U8" s="27">
+        <f>AA$17*Q8*AA$10*86400*12/1000000000*AA$7</f>
+        <v>0.38163176093442885</v>
+      </c>
+      <c r="V8" s="27">
+        <f>AA$12*U8*AA$14</f>
+        <v>3.8163176093442885</v>
+      </c>
+      <c r="W8">
+        <f>AA$16/H8</f>
+        <v>5.6197220480679224</v>
+      </c>
+      <c r="X8">
         <f t="shared" si="1"/>
-        <v>0.67807825935480448</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0.86776859504132231</v>
-      </c>
-      <c r="K8" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L8" s="27">
-        <f t="shared" si="4"/>
-        <v>1.4862789772321459</v>
-      </c>
-      <c r="M8" s="27">
-        <f t="shared" si="16"/>
-        <v>1.4862789772321459</v>
-      </c>
-      <c r="N8" s="27">
-        <f t="shared" si="17"/>
-        <v>1.2897462199121927</v>
-      </c>
-      <c r="O8" s="27">
-        <f t="shared" si="5"/>
-        <v>14.862789772321459</v>
-      </c>
-      <c r="P8" s="27">
-        <f t="shared" si="6"/>
-        <v>12.897462199121927</v>
-      </c>
-      <c r="Q8" s="27">
-        <f t="shared" si="7"/>
-        <v>1.7411011265922482</v>
-      </c>
-      <c r="R8" s="27">
-        <f t="shared" si="8"/>
-        <v>0.17411011265922482</v>
-      </c>
-      <c r="S8" s="27">
-        <f t="shared" si="18"/>
-        <v>22.495424991010037</v>
-      </c>
-      <c r="T8" s="27">
-        <f t="shared" si="19"/>
-        <v>20.530097417810502</v>
-      </c>
-      <c r="U8" s="27">
-        <f t="shared" si="20"/>
-        <v>0.76326352186885771</v>
-      </c>
-      <c r="V8" s="27">
-        <f t="shared" si="21"/>
-        <v>7.6326352186885771</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="9"/>
-        <v>4.29572376524413</v>
-      </c>
-      <c r="X8">
-        <f t="shared" si="10"/>
-        <v>17.523711481254221</v>
+        <v>14.055893642260905</v>
       </c>
       <c r="Z8" s="31" t="s">
         <v>30</v>
@@ -31945,100 +31982,100 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:30">
       <c r="A9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="12"/>
-        <v>35</v>
-      </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>(C9+ AA$2)/2</f>
         <v>26</v>
       </c>
       <c r="F9">
-        <f t="shared" si="13"/>
-        <v>5.6220563085635584</v>
+        <f t="shared" si="4"/>
+        <v>4.2426356531114431</v>
       </c>
       <c r="G9">
-        <f t="shared" si="14"/>
-        <v>2.3380938419374377</v>
+        <f t="shared" si="5"/>
+        <v>1.7052285488209411</v>
       </c>
       <c r="H9">
-        <f t="shared" si="15"/>
-        <v>3.2839624666261207</v>
+        <f t="shared" si="6"/>
+        <v>2.537407104290502</v>
       </c>
       <c r="I9">
+        <f>MAX(0, 1 - AA$8 * H9^ AA$9)</f>
+        <v>0.67807825935480448</v>
+      </c>
+      <c r="J9" s="27">
+        <f>IF(D9&lt;=$AA$2,MAX(0,(($AB$3-D9)*(D9-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D9)*(D9-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.96484375</v>
+      </c>
+      <c r="K9" s="27">
+        <f>IF(D9&gt;AA$2,1,MAX(0,((AA$3-D9)*(D9-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="27">
+        <f>AA$10*(AA$7*I9*AA$11*12)/1000000000</f>
+        <v>1.4862789772321459</v>
+      </c>
+      <c r="M9" s="27">
+        <f t="shared" si="7"/>
+        <v>1.4862789772321459</v>
+      </c>
+      <c r="N9" s="27">
+        <f t="shared" si="8"/>
+        <v>1.4340269819388283</v>
+      </c>
+      <c r="O9" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M9 * AA$14</f>
+        <v>14.862789772321459</v>
+      </c>
+      <c r="P9" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N9 * AA$14</f>
+        <v>14.340269819388283</v>
+      </c>
+      <c r="Q9" s="27">
+        <f>AA$18^((D9-AA$2)/10)</f>
+        <v>1.2311444133449163</v>
+      </c>
+      <c r="R9" s="27">
+        <f>AA$17*Q9</f>
+        <v>0.12311444133449163</v>
+      </c>
+      <c r="S9" s="27">
+        <f t="shared" si="9"/>
+        <v>20.259877893779418</v>
+      </c>
+      <c r="T9" s="27">
+        <f t="shared" si="10"/>
+        <v>19.737357940846241</v>
+      </c>
+      <c r="U9" s="27">
+        <f>AA$17*Q9*AA$10*86400*12/1000000000*AA$7</f>
+        <v>0.53970881214579591</v>
+      </c>
+      <c r="V9" s="27">
+        <f>AA$12*U9*AA$14</f>
+        <v>5.3970881214579594</v>
+      </c>
+      <c r="W9">
+        <f>AA$16/H9</f>
+        <v>4.29572376524413</v>
+      </c>
+      <c r="X9">
         <f t="shared" si="1"/>
-        <v>0.46077952588954418</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0.65082644628099173</v>
-      </c>
-      <c r="K9" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L9" s="27">
-        <f t="shared" si="4"/>
-        <v>1.0099821267242231</v>
-      </c>
-      <c r="M9" s="27">
-        <f t="shared" si="16"/>
-        <v>1.0099821267242231</v>
-      </c>
-      <c r="N9" s="27">
-        <f t="shared" si="17"/>
-        <v>0.65732307834324433</v>
-      </c>
-      <c r="O9" s="27">
-        <f t="shared" si="5"/>
-        <v>10.099821267242231</v>
-      </c>
-      <c r="P9" s="27">
-        <f t="shared" si="6"/>
-        <v>6.573230783432443</v>
-      </c>
-      <c r="Q9" s="27">
-        <f t="shared" si="7"/>
-        <v>2.4622888266898326</v>
-      </c>
-      <c r="R9" s="27">
-        <f t="shared" si="8"/>
-        <v>0.24622888266898327</v>
-      </c>
-      <c r="S9" s="27">
-        <f t="shared" si="18"/>
-        <v>20.893997510158151</v>
-      </c>
-      <c r="T9" s="27">
-        <f t="shared" si="19"/>
-        <v>17.36740702634836</v>
-      </c>
-      <c r="U9" s="27">
-        <f t="shared" si="20"/>
-        <v>1.0794176242915918</v>
-      </c>
-      <c r="V9" s="27">
-        <f t="shared" si="21"/>
-        <v>10.794176242915919</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="9"/>
-        <v>3.3191609559406592</v>
-      </c>
-      <c r="X9">
-        <f t="shared" si="10"/>
-        <v>19.185719907908702</v>
+        <v>16.847059169703542</v>
       </c>
       <c r="Z9" s="31" t="s">
         <v>31</v>
@@ -32047,100 +32084,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:30">
       <c r="A10">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="12"/>
-        <v>40</v>
-      </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f>(C10+ AA$2)/2</f>
         <v>28.5</v>
       </c>
       <c r="F10">
-        <f t="shared" si="13"/>
-        <v>7.3747231460360023</v>
+        <f t="shared" si="4"/>
+        <v>5.6220563085635584</v>
       </c>
       <c r="G10">
-        <f t="shared" si="14"/>
-        <v>3.1674898302368564</v>
+        <f t="shared" si="5"/>
+        <v>2.3380938419374377</v>
       </c>
       <c r="H10">
-        <f t="shared" si="15"/>
-        <v>4.2072333157991455</v>
+        <f t="shared" si="6"/>
+        <v>3.2839624666261207</v>
       </c>
       <c r="I10">
+        <f>MAX(0, 1 - AA$8 * H10^ AA$9)</f>
+        <v>0.46077952588954418</v>
+      </c>
+      <c r="J10" s="27">
+        <f>IF(D10&lt;=$AA$2,MAX(0,(($AB$3-D10)*(D10-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D10)*(D10-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.75</v>
+      </c>
+      <c r="K10" s="27">
+        <f>IF(D10&gt;AA$2,1,MAX(0,((AA$3-D10)*(D10-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>1</v>
+      </c>
+      <c r="L10" s="27">
+        <f>AA$10*(AA$7*I10*AA$11*12)/1000000000</f>
+        <v>1.0099821267242231</v>
+      </c>
+      <c r="M10" s="27">
+        <f t="shared" si="7"/>
+        <v>1.0099821267242231</v>
+      </c>
+      <c r="N10" s="27">
+        <f t="shared" si="8"/>
+        <v>0.75748659504316729</v>
+      </c>
+      <c r="O10" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M10 * AA$14</f>
+        <v>10.099821267242231</v>
+      </c>
+      <c r="P10" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N10 * AA$14</f>
+        <v>7.5748659504316729</v>
+      </c>
+      <c r="Q10" s="27">
+        <f>AA$18^((D10-AA$2)/10)</f>
+        <v>1.7411011265922482</v>
+      </c>
+      <c r="R10" s="27">
+        <f>AA$17*Q10</f>
+        <v>0.17411011265922482</v>
+      </c>
+      <c r="S10" s="27">
+        <f t="shared" si="9"/>
+        <v>17.732456485930808</v>
+      </c>
+      <c r="T10" s="27">
+        <f t="shared" si="10"/>
+        <v>15.207501169120249</v>
+      </c>
+      <c r="U10" s="27">
+        <f>AA$17*Q10*AA$10*86400*12/1000000000*AA$7</f>
+        <v>0.76326352186885771</v>
+      </c>
+      <c r="V10" s="27">
+        <f>AA$12*U10*AA$14</f>
+        <v>7.6326352186885771</v>
+      </c>
+      <c r="W10">
+        <f>AA$16/H10</f>
+        <v>3.3191609559406592</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="1"/>
-        <v>0.11495939132148625</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
-        <v>0.33057851239669422</v>
-      </c>
-      <c r="K10" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L10" s="27">
-        <f t="shared" si="4"/>
-        <v>0.25197936108304753</v>
-      </c>
-      <c r="M10" s="27">
-        <f t="shared" si="16"/>
-        <v>0.25197936108304753</v>
-      </c>
-      <c r="N10" s="27">
-        <f t="shared" si="17"/>
-        <v>8.3298962341503316E-2</v>
-      </c>
-      <c r="O10" s="27">
-        <f t="shared" si="5"/>
-        <v>2.519793610830475</v>
-      </c>
-      <c r="P10" s="27">
-        <f t="shared" si="6"/>
-        <v>0.83298962341503313</v>
-      </c>
-      <c r="Q10" s="27">
-        <f t="shared" si="7"/>
-        <v>3.4822022531844965</v>
-      </c>
-      <c r="R10" s="27">
-        <f t="shared" si="8"/>
-        <v>0.34822022531844965</v>
-      </c>
-      <c r="S10" s="27">
-        <f t="shared" si="18"/>
-        <v>17.78506404820763</v>
-      </c>
-      <c r="T10" s="27">
-        <f t="shared" si="19"/>
-        <v>16.098260060792189</v>
-      </c>
-      <c r="U10" s="27">
-        <f t="shared" si="20"/>
-        <v>1.5265270437377154</v>
-      </c>
-      <c r="V10" s="27">
-        <f t="shared" si="21"/>
-        <v>15.265270437377154</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="9"/>
-        <v>2.5907762136860701</v>
-      </c>
-      <c r="X10">
-        <f t="shared" si="10"/>
-        <v>22.783501424948021</v>
+        <v>16.799678702024501</v>
       </c>
       <c r="Z10" s="31" t="s">
         <v>10</v>
@@ -32152,100 +32189,100 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:30">
       <c r="A11">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:C13" si="22">(A11+B11)/2</f>
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="12"/>
-        <v>45</v>
-      </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f>(C11+ AA$2)/2</f>
         <v>31</v>
       </c>
       <c r="F11">
-        <f t="shared" si="13"/>
-        <v>9.5812372781996284</v>
+        <f t="shared" si="4"/>
+        <v>7.3747231460360023</v>
       </c>
       <c r="G11">
-        <f t="shared" si="14"/>
-        <v>4.2426356531114431</v>
+        <f t="shared" si="5"/>
+        <v>3.1674898302368564</v>
       </c>
       <c r="H11">
-        <f t="shared" si="15"/>
-        <v>5.3386016250881854</v>
+        <f t="shared" si="6"/>
+        <v>4.2072333157991455</v>
       </c>
       <c r="I11">
+        <f>MAX(0, 1 - AA$8 * H11^ AA$9)</f>
+        <v>0.11495939132148625</v>
+      </c>
+      <c r="J11" s="27">
+        <f>IF(D11&lt;=$AA$2,MAX(0,(($AB$3-D11)*(D11-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D11)*(D11-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0.33984375</v>
+      </c>
+      <c r="K11" s="27">
+        <f>IF(D11&gt;AA$2,1,MAX(0,((AA$3-D11)*(D11-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>1</v>
+      </c>
+      <c r="L11" s="27">
+        <f>AA$10*(AA$7*I11*AA$11*12)/1000000000</f>
+        <v>0.25197936108304753</v>
+      </c>
+      <c r="M11" s="27">
+        <f t="shared" si="7"/>
+        <v>0.25197936108304753</v>
+      </c>
+      <c r="N11" s="27">
+        <f t="shared" si="8"/>
+        <v>8.5633610993066933E-2</v>
+      </c>
+      <c r="O11" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M11 * AA$14</f>
+        <v>2.519793610830475</v>
+      </c>
+      <c r="P11" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N11 * AA$14</f>
+        <v>0.85633610993066933</v>
+      </c>
+      <c r="Q11" s="27">
+        <f>AA$18^((D11-AA$2)/10)</f>
+        <v>2.4622888266898326</v>
+      </c>
+      <c r="R11" s="27">
+        <f>AA$17*Q11</f>
+        <v>0.24622888266898327</v>
+      </c>
+      <c r="S11" s="27">
+        <f t="shared" si="9"/>
+        <v>13.313969853746393</v>
+      </c>
+      <c r="T11" s="27">
+        <f t="shared" si="10"/>
+        <v>11.650512352846588</v>
+      </c>
+      <c r="U11" s="27">
+        <f>AA$17*Q11*AA$10*86400*12/1000000000*AA$7</f>
+        <v>1.0794176242915918</v>
+      </c>
+      <c r="V11" s="27">
+        <f>AA$12*U11*AA$14</f>
+        <v>10.794176242915919</v>
+      </c>
+      <c r="W11">
+        <f>AA$16/H11</f>
+        <v>2.5907762136860701</v>
+      </c>
+      <c r="X11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L11" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="27">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="27">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="27">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="27">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="27">
-        <f t="shared" si="7"/>
-        <v>4.9245776533796644</v>
-      </c>
-      <c r="R11" s="27">
-        <f t="shared" si="8"/>
-        <v>0.49245776533796648</v>
-      </c>
-      <c r="S11" s="27">
-        <f t="shared" si="18"/>
-        <v>21.588352485831837</v>
-      </c>
-      <c r="T11" s="27">
-        <f t="shared" si="19"/>
-        <v>21.588352485831837</v>
-      </c>
-      <c r="U11" s="27">
-        <f t="shared" si="20"/>
-        <v>2.1588352485831837</v>
-      </c>
-      <c r="V11" s="27">
-        <f t="shared" si="21"/>
-        <v>21.588352485831837</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="9"/>
-        <v>2.0417331663738723</v>
-      </c>
-      <c r="X11">
-        <f t="shared" si="10"/>
-        <v>38.769655972545031</v>
+        <v>16.48870522591077</v>
       </c>
       <c r="Z11" s="31" t="s">
         <v>11</v>
@@ -32261,100 +32298,100 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:30">
       <c r="A12">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C12">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="C12:C14" si="11">(A12+B12)/2</f>
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="12"/>
-        <v>50</v>
-      </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>(C12+ AA$2)/2</f>
         <v>33.5</v>
       </c>
       <c r="F12">
-        <f t="shared" si="13"/>
-        <v>12.335046017492973</v>
+        <f t="shared" si="4"/>
+        <v>9.5812372781996284</v>
       </c>
       <c r="G12">
-        <f t="shared" si="14"/>
-        <v>5.6220563085635584</v>
+        <f t="shared" si="5"/>
+        <v>4.2426356531114431</v>
       </c>
       <c r="H12">
-        <f t="shared" si="15"/>
-        <v>6.7129897089294142</v>
+        <f t="shared" si="6"/>
+        <v>5.3386016250881854</v>
       </c>
       <c r="I12">
+        <f>MAX(0, 1 - AA$8 * H12^ AA$9)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="27">
+        <f>IF(D12&lt;=$AA$2,MAX(0,(($AB$3-D12)*(D12-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D12)*(D12-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="27">
+        <f>IF(D12&gt;AA$2,1,MAX(0,((AA$3-D12)*(D12-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="27">
+        <f>AA$10*(AA$7*I12*AA$11*12)/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M12 * AA$14</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N12 * AA$14</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="27">
+        <f>AA$18^((D12-AA$2)/10)</f>
+        <v>3.4822022531844965</v>
+      </c>
+      <c r="R12" s="27">
+        <f>AA$17*Q12</f>
+        <v>0.34822022531844965</v>
+      </c>
+      <c r="S12" s="27">
+        <f t="shared" si="9"/>
+        <v>15.265270437377154</v>
+      </c>
+      <c r="T12" s="27">
+        <f t="shared" si="10"/>
+        <v>15.265270437377154</v>
+      </c>
+      <c r="U12" s="27">
+        <f>AA$17*Q12*AA$10*86400*12/1000000000*AA$7</f>
+        <v>1.5265270437377154</v>
+      </c>
+      <c r="V12" s="27">
+        <f>AA$12*U12*AA$14</f>
+        <v>15.265270437377154</v>
+      </c>
+      <c r="W12">
+        <f>AA$16/H12</f>
+        <v>2.0417331663738723</v>
+      </c>
+      <c r="X12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="27">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="27">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="27">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="27">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="27">
-        <f t="shared" si="7"/>
-        <v>6.9644045063689921</v>
-      </c>
-      <c r="R12" s="27">
-        <f t="shared" si="8"/>
-        <v>0.6964404506368993</v>
-      </c>
-      <c r="S12" s="27">
-        <f t="shared" si="18"/>
-        <v>30.530540874754308</v>
-      </c>
-      <c r="T12" s="27">
-        <f t="shared" si="19"/>
-        <v>30.530540874754308</v>
-      </c>
-      <c r="U12" s="27">
-        <f t="shared" si="20"/>
-        <v>3.0530540874754308</v>
-      </c>
-      <c r="V12" s="27">
-        <f t="shared" si="21"/>
-        <v>30.530540874754308</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="9"/>
-        <v>1.6237176686717028</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="10"/>
-        <v>68.943831000092331</v>
+        <v>27.414286642456123</v>
       </c>
       <c r="Z12" s="31" t="s">
         <v>20</v>
@@ -32363,100 +32400,100 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:30">
       <c r="A13">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="11"/>
+        <v>45</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="12"/>
-        <v>55</v>
-      </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>(C13+ AA$2)/2</f>
         <v>36</v>
       </c>
       <c r="F13">
-        <f t="shared" si="13"/>
-        <v>15.743681776119971</v>
+        <f t="shared" si="4"/>
+        <v>12.335046017492973</v>
       </c>
       <c r="G13">
-        <f t="shared" si="14"/>
-        <v>7.3747231460360023</v>
+        <f t="shared" si="5"/>
+        <v>5.6220563085635584</v>
       </c>
       <c r="H13">
-        <f t="shared" si="15"/>
-        <v>8.3689586300839682</v>
+        <f t="shared" si="6"/>
+        <v>6.7129897089294142</v>
       </c>
       <c r="I13">
+        <f>MAX(0, 1 - AA$8 * H13^ AA$9)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="27">
+        <f>IF(D13&lt;=$AA$2,MAX(0,(($AB$3-D13)*(D13-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D13)*(D13-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="27">
+        <f>IF(D13&gt;AA$2,1,MAX(0,((AA$3-D13)*(D13-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="27">
+        <f>AA$10*(AA$7*I13*AA$11*12)/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M13 * AA$14</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N13 * AA$14</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="27">
+        <f>AA$18^((D13-AA$2)/10)</f>
+        <v>4.9245776533796644</v>
+      </c>
+      <c r="R13" s="27">
+        <f>AA$17*Q13</f>
+        <v>0.49245776533796648</v>
+      </c>
+      <c r="S13" s="27">
+        <f t="shared" si="9"/>
+        <v>21.588352485831837</v>
+      </c>
+      <c r="T13" s="27">
+        <f t="shared" si="10"/>
+        <v>21.588352485831837</v>
+      </c>
+      <c r="U13" s="27">
+        <f>AA$17*Q13*AA$10*86400*12/1000000000*AA$7</f>
+        <v>2.1588352485831837</v>
+      </c>
+      <c r="V13" s="27">
+        <f>AA$12*U13*AA$14</f>
+        <v>21.588352485831837</v>
+      </c>
+      <c r="W13">
+        <f>AA$16/H13</f>
+        <v>1.6237176686717028</v>
+      </c>
+      <c r="X13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L13" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="27">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="27">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="27">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="27">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="27">
-        <f t="shared" si="7"/>
-        <v>9.8491553067593287</v>
-      </c>
-      <c r="R13" s="27">
-        <f t="shared" si="8"/>
-        <v>0.98491553067593296</v>
-      </c>
-      <c r="S13" s="27">
-        <f t="shared" si="18"/>
-        <v>43.176704971663675</v>
-      </c>
-      <c r="T13" s="27">
-        <f t="shared" si="19"/>
-        <v>43.176704971663675</v>
-      </c>
-      <c r="U13" s="27">
-        <f t="shared" si="20"/>
-        <v>4.3176704971663673</v>
-      </c>
-      <c r="V13" s="27">
-        <f t="shared" si="21"/>
-        <v>43.176704971663675</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="9"/>
-        <v>1.3024320565784224</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="10"/>
-        <v>121.55304692975949</v>
+        <v>48.750650421144599</v>
       </c>
       <c r="Z13" s="31" t="s">
         <v>21</v>
@@ -32465,7 +32502,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:30">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="E14">
+        <f>(C14+ AA$2)/2</f>
+        <v>38.5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>15.743681776119971</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>7.3747231460360023</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>8.3689586300839682</v>
+      </c>
+      <c r="I14">
+        <f>MAX(0, 1 - AA$8 * H14^ AA$9)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="27">
+        <f>IF(D14&lt;=$AA$2,MAX(0,(($AB$3-D14)*(D14-$AA$1))/((($AB$3-$AA$1)/2)^2)),MAX(0,(($AA$3-D14)*(D14-$AB$1))/((($AA$3-$AB$1)/2)^2)))</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="27">
+        <f>IF(D14&gt;AA$2,1,MAX(0,((AA$3-D14)*(D14-AA$1))/(((AA$3-AA$1)/2)^2)))</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="27">
+        <f>AA$10*(AA$7*I14*AA$11*12)/1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="27">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="27">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* M14 * AA$14</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="27">
+        <f xml:space="preserve"> AA$12*AA$13* N14 * AA$14</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="27">
+        <f>AA$18^((D14-AA$2)/10)</f>
+        <v>6.9644045063689921</v>
+      </c>
+      <c r="R14" s="27">
+        <f>AA$17*Q14</f>
+        <v>0.6964404506368993</v>
+      </c>
+      <c r="S14" s="27">
+        <f t="shared" si="9"/>
+        <v>30.530540874754308</v>
+      </c>
+      <c r="T14" s="27">
+        <f t="shared" si="10"/>
+        <v>30.530540874754308</v>
+      </c>
+      <c r="U14" s="27">
+        <f>AA$17*Q14*AA$10*86400*12/1000000000*AA$7</f>
+        <v>3.0530540874754308</v>
+      </c>
+      <c r="V14" s="27">
+        <f>AA$12*U14*AA$14</f>
+        <v>30.530540874754308</v>
+      </c>
+      <c r="W14">
+        <f>AA$16/H14</f>
+        <v>1.3024320565784224</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="1"/>
+        <v>85.950983757919587</v>
+      </c>
       <c r="Z14" s="31" t="s">
         <v>24</v>
       </c>
@@ -32473,7 +32604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:30">
       <c r="Z15" s="31" t="s">
         <v>25</v>
       </c>
@@ -32481,7 +32612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:30">
       <c r="Z16" s="31" t="s">
         <v>33</v>
       </c>
@@ -32498,16 +32629,18 @@
       </c>
     </row>
     <row r="18" spans="19:27">
-      <c r="S18" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="T18" s="2"/>
       <c r="Z18" s="31" t="s">
         <v>147</v>
       </c>
       <c r="AA18" s="31">
         <v>2</v>
       </c>
+    </row>
+    <row r="19" spans="19:27">
+      <c r="S19" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="T19" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -32525,14 +32658,14 @@
       <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="9.109375" style="27"/>
-    <col min="9" max="17" width="9.109375" style="4"/>
-    <col min="18" max="18" width="12.5546875" customWidth="1"/>
-    <col min="22" max="22" width="9.109375" style="4"/>
-    <col min="25" max="25" width="10.44140625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="8.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="27"/>
+    <col min="9" max="17" width="9.140625" style="4"/>
+    <col min="18" max="18" width="12.5703125" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="4"/>
+    <col min="25" max="25" width="10.42578125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -33800,14 +33933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" style="27" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="27"/>
+    <col min="2" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -34025,9 +34158,9 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.109375" style="27"/>
+    <col min="2" max="2" width="9.140625" style="27"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -34361,7 +34494,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="27" t="s">
@@ -35059,9 +35192,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -35107,7 +35240,7 @@
         <v>0.84029689765843141</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6">
+    <row r="5" spans="1:9" ht="15.75">
       <c r="A5" s="27">
         <f t="shared" si="1"/>
         <v>4300</v>
@@ -35373,18 +35506,18 @@
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="27"/>
-    <col min="3" max="3" width="10.33203125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="27"/>
+    <col min="3" max="3" width="10.28515625" style="27" customWidth="1"/>
     <col min="4" max="4" width="11" style="27" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="27" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" style="27" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="27" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="27"/>
-    <col min="9" max="9" width="10.109375" style="27" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="27"/>
+    <col min="5" max="5" width="11.5703125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="27" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="27"/>
+    <col min="9" max="9" width="10.140625" style="27" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">

</xml_diff>